<commit_message>
feat:more full desc and trans
</commit_message>
<xml_diff>
--- a/transData.xlsx
+++ b/transData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ドキュメント\VisualStudioProject\AmongUs\ExtremeRoles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4077D51D-207C-4F91-A447-A032C5BB2C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50901E9C-F0D0-438C-95E4-22D34115FB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="614">
   <si>
     <t>English</t>
   </si>
@@ -2411,9 +2411,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Maintainer</t>
-  </si>
-  <si>
     <t>MaintainerSpawnRate</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -3089,6 +3086,1199 @@
     <t>のロール設定</t>
     <rPh sb="4" eb="6">
       <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SpecialCrewFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SheriffFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>キルが可能なクルー役職。ただし、キル可能回数には上限がある
+キルを行おうとした相手がクルー役職であればキルは失敗して死亡する</t>
+    <rPh sb="3" eb="5">
+      <t>カノウ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>カノウ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>カイスウ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ジョウゲン</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>アイテ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>シッパイ</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>シボウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Maintainer</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MaintainerFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Extreme Rolesの各役職の共通設定が適用できるクルー役職
+設定内容は以下を確認</t>
+    <rPh sb="14" eb="17">
+      <t>カクヤクショク</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>キョウツウ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>テキヨウ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="34" eb="38">
+      <t>セッテイナイヨウ</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>緊急修理が行えるクルー役職
+緊急修理は緊急タスク(サボタージ)発生時、使用可能
+緊急修理が発動すると緊急タスクはすぐに完了し、マップ内のドアが全て開きます</t>
+    <rPh sb="0" eb="2">
+      <t>キンキュウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>シュウリ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="14" eb="18">
+      <t>キンキュウ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>キンキュウ</t>
+    </rPh>
+    <rPh sb="31" eb="34">
+      <t>ハッセイジ</t>
+    </rPh>
+    <rPh sb="35" eb="39">
+      <t>シヨウカノウ</t>
+    </rPh>
+    <rPh sb="40" eb="44">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ハツドウ</t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t>キンキュウ</t>
+    </rPh>
+    <rPh sb="59" eb="61">
+      <t>カンリョウ</t>
+    </rPh>
+    <rPh sb="66" eb="67">
+      <t>ナイ</t>
+    </rPh>
+    <rPh sb="71" eb="72">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="73" eb="74">
+      <t>ヒラ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NeetFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>何も出来ないクルー役職
+何もしなくていいので、監視役に向いているかも？</t>
+    <rPh sb="0" eb="1">
+      <t>ナニ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>デキ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>ナニ</t>
+    </rPh>
+    <rPh sb="23" eb="26">
+      <t>カンシヤク</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>ム</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SpecialImpostorFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Extreme Rolesの各役職の共通設定が適用できるインポスター役職
+設定内容は以下を確認</t>
+    <rPh sb="14" eb="17">
+      <t>カクヤクショク</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>キョウツウ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>テキヨウ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="37" eb="41">
+      <t>セッテイナイヨウ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>EvolverFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CarrierFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>死体を運ぶことができるインポスター役職
+「キャリー」の発動時間が切れると死体をその場に落とす</t>
+    <rPh sb="0" eb="2">
+      <t>シタイ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ハコ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ハツドウ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>ジカン</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>シタイ</t>
+    </rPh>
+    <rPh sb="41" eb="42">
+      <t>バ</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>オ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>死体を喰うことで、キルクールタイムが短くなるインポスター役職
+捕食中は死体の近くに居なければならない
+捕食後は新しいキルクールタイムが適用される</t>
+    <rPh sb="0" eb="2">
+      <t>シタイ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ク</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>ミジカ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>ホショク</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>チュウ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>シタイ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>チカ</t>
+    </rPh>
+    <rPh sb="41" eb="42">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>ホショク</t>
+    </rPh>
+    <rPh sb="53" eb="54">
+      <t>ゴ</t>
+    </rPh>
+    <rPh sb="55" eb="56">
+      <t>アタラ</t>
+    </rPh>
+    <rPh sb="67" eb="69">
+      <t>テキヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AliceFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>JackalFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>第三陣営役職
+勝利条件1：インポスターにキルされる
+勝利条件2：自分以外の生存者が一人でクルー役職かインポスター役職
+会議で追放された場合、敗北
+「破壊工作」により完了しているタスクの一部がリセットされる
+強力な役職のためインポスター及びクルー両方狙われるため注意が必要</t>
+    <rPh sb="0" eb="4">
+      <t>ダイサンジ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="7" eb="11">
+      <t>ショウリジョウケン</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ショウリ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>ジョウケン</t>
+    </rPh>
+    <rPh sb="32" eb="36">
+      <t>ジブンイガイ</t>
+    </rPh>
+    <rPh sb="37" eb="40">
+      <t>セイゾンシャ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>ヒトリ</t>
+    </rPh>
+    <rPh sb="56" eb="58">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="59" eb="61">
+      <t>カイギ</t>
+    </rPh>
+    <rPh sb="62" eb="64">
+      <t>ツイホウ</t>
+    </rPh>
+    <rPh sb="67" eb="69">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="70" eb="72">
+      <t>ハイボク</t>
+    </rPh>
+    <rPh sb="74" eb="78">
+      <t>ハカイ</t>
+    </rPh>
+    <rPh sb="82" eb="84">
+      <t>カンリョウ</t>
+    </rPh>
+    <rPh sb="92" eb="94">
+      <t>イチブ</t>
+    </rPh>
+    <rPh sb="103" eb="105">
+      <t>キョウリョク</t>
+    </rPh>
+    <rPh sb="106" eb="108">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="117" eb="118">
+      <t>オヨ</t>
+    </rPh>
+    <rPh sb="122" eb="124">
+      <t>リョウホウ</t>
+    </rPh>
+    <rPh sb="124" eb="125">
+      <t>ネラ</t>
+    </rPh>
+    <rPh sb="130" eb="132">
+      <t>チュウイ</t>
+    </rPh>
+    <rPh sb="133" eb="135">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NeetNeutralFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>何も出来ない第三陣営役職
+勝利条件：生き残っていること
+何もしなくていいので、監視役に向いているかも？</t>
+    <rPh sb="0" eb="1">
+      <t>ナニ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>デキ</t>
+    </rPh>
+    <rPh sb="6" eb="10">
+      <t>ダイサンジ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="13" eb="17">
+      <t>ショウリジョウケン</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ノコ</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>ナニ</t>
+    </rPh>
+    <rPh sb="39" eb="42">
+      <t>カンシヤク</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>ム</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>第三陣営役職
+勝利条件：インポスター及びキル能力を持つ第三陣営が全滅しており、
+生存者の半数以上が同じ陣営。
+「サイドキック」を使うことで任意の人を同じ陣営に引き込むことが可能
+「サイドキック」の対象になった人は「サイドキック」という役職になる</t>
+    <rPh sb="0" eb="1">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ジンエイ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="7" eb="11">
+      <t>ショウリジョウケン</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>オヨ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ノウリョク</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="27" eb="31">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>ゼンメツ</t>
+    </rPh>
+    <rPh sb="40" eb="43">
+      <t>セイゾンシャ</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>ハンスウ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="49" eb="50">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>ジンエイ</t>
+    </rPh>
+    <rPh sb="64" eb="65">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="69" eb="71">
+      <t>ニンイ</t>
+    </rPh>
+    <rPh sb="72" eb="73">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="74" eb="75">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="76" eb="78">
+      <t>ジンエイ</t>
+    </rPh>
+    <rPh sb="79" eb="80">
+      <t>ヒ</t>
+    </rPh>
+    <rPh sb="81" eb="82">
+      <t>コ</t>
+    </rPh>
+    <rPh sb="86" eb="88">
+      <t>カノウ</t>
+    </rPh>
+    <rPh sb="98" eb="100">
+      <t>タイショウ</t>
+    </rPh>
+    <rPh sb="104" eb="105">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="117" eb="119">
+      <t>ヤクショク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MarlinFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AssassinFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>インポスター陣営に新しい勝利条件を追加するインポスター役職
+新しい勝利条件：アサシンの特殊能力でマーリンを当てる
+アサシンの特殊能力：マーリン指定の特殊会議
+マーリン指定の特殊会議：全員が参加するが能力を発動させたアサシン以外投票不可
+　　　　　　　　　　　　スキップ不可、チャット不可、死亡している人にも投票可
+　　　　　　　　　　　　投票先がマーリンであればインポスター勝利、それ以外の
+　　　　　　　　　　　　場合、ゲームが続行(マーリンの能力は継続)
+特殊能力発動条件：追放された場合、自身がキルされた場合の処理は設定可
+上記の能力以外は普通のインポスターのため、マーリンを探りつつ潜伏しキルを行う必要がある</t>
+    <rPh sb="6" eb="8">
+      <t>ジンエイ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>アタラ</t>
+    </rPh>
+    <rPh sb="12" eb="16">
+      <t>ショウリジョウケン</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ツイカ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>アタラ</t>
+    </rPh>
+    <rPh sb="43" eb="47">
+      <t>トクシュノウリョク</t>
+    </rPh>
+    <rPh sb="53" eb="54">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="62" eb="66">
+      <t>トク</t>
+    </rPh>
+    <rPh sb="71" eb="73">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="74" eb="76">
+      <t>トクシュ</t>
+    </rPh>
+    <rPh sb="76" eb="78">
+      <t>カイギ</t>
+    </rPh>
+    <rPh sb="83" eb="85">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="86" eb="88">
+      <t>トクシュ</t>
+    </rPh>
+    <rPh sb="88" eb="90">
+      <t>カイギ</t>
+    </rPh>
+    <rPh sb="91" eb="93">
+      <t>ゼンイン</t>
+    </rPh>
+    <rPh sb="94" eb="96">
+      <t>サンカ</t>
+    </rPh>
+    <rPh sb="99" eb="101">
+      <t>ノウリョク</t>
+    </rPh>
+    <rPh sb="102" eb="104">
+      <t>ハツドウ</t>
+    </rPh>
+    <rPh sb="111" eb="113">
+      <t>イガイ</t>
+    </rPh>
+    <rPh sb="113" eb="115">
+      <t>トウヒョウ</t>
+    </rPh>
+    <rPh sb="115" eb="117">
+      <t>フカ</t>
+    </rPh>
+    <rPh sb="134" eb="136">
+      <t>フカ</t>
+    </rPh>
+    <rPh sb="141" eb="143">
+      <t>フカ</t>
+    </rPh>
+    <rPh sb="144" eb="146">
+      <t>シボウ</t>
+    </rPh>
+    <rPh sb="150" eb="151">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="153" eb="155">
+      <t>トウヒョウ</t>
+    </rPh>
+    <rPh sb="155" eb="156">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="169" eb="171">
+      <t>トウヒョウ</t>
+    </rPh>
+    <rPh sb="171" eb="172">
+      <t>サキ</t>
+    </rPh>
+    <rPh sb="187" eb="189">
+      <t>ショウリ</t>
+    </rPh>
+    <rPh sb="192" eb="194">
+      <t>イガイ</t>
+    </rPh>
+    <rPh sb="208" eb="210">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="215" eb="217">
+      <t>ゾッコウ</t>
+    </rPh>
+    <rPh sb="223" eb="225">
+      <t>ノウリョク</t>
+    </rPh>
+    <rPh sb="226" eb="228">
+      <t>ケイゾク</t>
+    </rPh>
+    <rPh sb="230" eb="234">
+      <t>トクシュ</t>
+    </rPh>
+    <rPh sb="234" eb="238">
+      <t>ハツドウジョウケン</t>
+    </rPh>
+    <rPh sb="239" eb="241">
+      <t>ツイホウ</t>
+    </rPh>
+    <rPh sb="244" eb="246">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="255" eb="257">
+      <t>バアイショリ</t>
+    </rPh>
+    <rPh sb="265" eb="267">
+      <t>ジョウキ</t>
+    </rPh>
+    <rPh sb="268" eb="270">
+      <t>ノウリョク</t>
+    </rPh>
+    <rPh sb="270" eb="272">
+      <t>イガイ</t>
+    </rPh>
+    <rPh sb="273" eb="275">
+      <t>フツウ</t>
+    </rPh>
+    <rPh sb="291" eb="292">
+      <t>サグ</t>
+    </rPh>
+    <rPh sb="295" eb="297">
+      <t>センプク</t>
+    </rPh>
+    <rPh sb="301" eb="302">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="303" eb="305">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>インポスターが誰か分かるクルー役職
+アサシンの特殊能力によって指定された場合、クルー全体の敗北
+インポスターが分かるので会議を主導しつつ、身を隠す必要がある
+インポスターに近い設定の役職のため、注意が必要</t>
+    <rPh sb="7" eb="8">
+      <t>ダレ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>ワ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="23" eb="27">
+      <t>トクシュノウリョク</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>ゼンタイ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ハイボク</t>
+    </rPh>
+    <rPh sb="55" eb="56">
+      <t>ワ</t>
+    </rPh>
+    <rPh sb="60" eb="62">
+      <t>カイギ</t>
+    </rPh>
+    <rPh sb="63" eb="65">
+      <t>シュドウ</t>
+    </rPh>
+    <rPh sb="69" eb="70">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="71" eb="72">
+      <t>カク</t>
+    </rPh>
+    <rPh sb="73" eb="75">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="86" eb="87">
+      <t>チカ</t>
+    </rPh>
+    <rPh sb="88" eb="90">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="91" eb="93">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="97" eb="99">
+      <t>チュウイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LoverFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LoverNeutralFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LoverImposterFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>複数人1組の第三陣営役職
+勝利条件1：生存者が同じ組以下になること
+勝利条件2：同じ組のタスクが全て終了すること
+同じ組の人が一定数以下になると自決する
+自決を行う人数は設定により変化する</t>
+    <rPh sb="0" eb="3">
+      <t>フクスウニン</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>クミ</t>
+    </rPh>
+    <rPh sb="6" eb="10">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="13" eb="17">
+      <t>ショウリジョウケン</t>
+    </rPh>
+    <rPh sb="19" eb="22">
+      <t>セイゾンシャ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>クミ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>クミ</t>
+    </rPh>
+    <rPh sb="48" eb="49">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t>シュウリョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>複数人1組のインポスター役職
+勝利条件1：インポスター勝利、ただし、同じ組は敗北
+勝利条件2：同じ組のタスクが全て終了すること
+勝利条件3：生存者が同じ組以下になること
+同じ組の人が一定数以下になると自決もしくは第三陣営に変化する
+自決を行う人数は設定により変化する</t>
+    <rPh sb="0" eb="3">
+      <t>フクスウニン</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>クミ</t>
+    </rPh>
+    <rPh sb="15" eb="19">
+      <t>ショウリジョウケン</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ショウリ</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>ハイボク</t>
+    </rPh>
+    <rPh sb="41" eb="45">
+      <t>ショウリ</t>
+    </rPh>
+    <rPh sb="64" eb="68">
+      <t>ショウリ</t>
+    </rPh>
+    <rPh sb="85" eb="86">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="87" eb="88">
+      <t>クミ</t>
+    </rPh>
+    <rPh sb="89" eb="90">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="91" eb="94">
+      <t>イッテイスウ</t>
+    </rPh>
+    <rPh sb="94" eb="96">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="100" eb="102">
+      <t>ジケツ</t>
+    </rPh>
+    <rPh sb="106" eb="110">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="111" eb="113">
+      <t>ヘンカ</t>
+    </rPh>
+    <rPh sb="116" eb="118">
+      <t>ジケツ</t>
+    </rPh>
+    <rPh sb="119" eb="120">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="121" eb="123">
+      <t>ニンズウ</t>
+    </rPh>
+    <rPh sb="124" eb="126">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="129" eb="131">
+      <t>ヘンカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>複数人1組のクルー役職
+勝利条件1：クルー勝利、ただし、同じ組で別陣営の人が居た場合その人は敗北
+勝利条件2：生存者が同じ組以下になること
+同じ組の人が一定数以下になると自決もしくは第三陣営に変化する
+自決を行う人数は設定により変化する</t>
+    <rPh sb="0" eb="3">
+      <t>フクスウニン</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>クミ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>ベツ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ジンエイ</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="70" eb="71">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="72" eb="73">
+      <t>クミ</t>
+    </rPh>
+    <rPh sb="74" eb="75">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="76" eb="79">
+      <t>イッテイスウ</t>
+    </rPh>
+    <rPh sb="79" eb="81">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="85" eb="87">
+      <t>ジケツ</t>
+    </rPh>
+    <rPh sb="91" eb="95">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="96" eb="98">
+      <t>ヘンカ</t>
+    </rPh>
+    <rPh sb="101" eb="103">
+      <t>ジケツ</t>
+    </rPh>
+    <rPh sb="104" eb="105">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="106" eb="108">
+      <t>ニンズウ</t>
+    </rPh>
+    <rPh sb="109" eb="111">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="114" eb="116">
+      <t>ヘンカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LoverNeutralKillerFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>相方を殺された恨みで殺人鬼に変化した複数人1組の第三陣営役職
+勝利条件：生存者が同じ組以下になること</t>
+    <rPh sb="3" eb="4">
+      <t>コロ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ウラ</t>
+    </rPh>
+    <rPh sb="10" eb="13">
+      <t>サツジンキ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ヘンカ</t>
+    </rPh>
+    <rPh sb="18" eb="21">
+      <t>フクスウニン</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>クミ</t>
+    </rPh>
+    <rPh sb="24" eb="28">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="31" eb="35">
+      <t>ショウリジョウケン</t>
+    </rPh>
+    <rPh sb="36" eb="39">
+      <t>セイゾンシャ</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>クミ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>イカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SupporterFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ゲーム開始時、一人だけ役職を知っているクルー役職
+1人だけ役職が分かるためその人をサポートする必要がある
+誰かにマーリンがアサインされている場合、マーリンがサポート対象となる
+それ以外だと、クルー陣営からランダムにサポート対象が決定される</t>
+    <rPh sb="3" eb="6">
+      <t>カイシジ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ヒトリ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>シ</t>
+    </rPh>
+    <rPh sb="21" eb="24">
+      <t>^</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>ワ</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="47" eb="49">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="53" eb="54">
+      <t>ダレ</t>
+    </rPh>
+    <rPh sb="70" eb="72">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="82" eb="84">
+      <t>タイショウ</t>
+    </rPh>
+    <rPh sb="90" eb="92">
+      <t>イガイ</t>
+    </rPh>
+    <rPh sb="98" eb="100">
+      <t>ジンエイ</t>
+    </rPh>
+    <rPh sb="114" eb="116">
+      <t>ケッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SupporterImposterFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ゲーム開始時、一人だけ役職を知っているインポスター役職
+1人だけ役職が分かるためその人をサポートする必要がある
+誰かにアサシンがアサインされている場合、アサシンがサポート対象となる
+それ以外だと、インポスター陣営からランダムにサポート対象が決定される</t>
+    <rPh sb="3" eb="6">
+      <t>カイシジ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ヒトリ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>シ</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>ワ</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="56" eb="57">
+      <t>ダレ</t>
+    </rPh>
+    <rPh sb="73" eb="75">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="85" eb="87">
+      <t>タイショウ</t>
+    </rPh>
+    <rPh sb="93" eb="95">
+      <t>イガイ</t>
+    </rPh>
+    <rPh sb="104" eb="106">
+      <t>ジンエイ</t>
+    </rPh>
+    <rPh sb="120" eb="122">
+      <t>ケッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ジャッカルのアシストを行う第三陣営役職
+勝利条件：インポスター及びキル能力を持つ第三陣営が全滅しており、
+生存者の半数以上が同じ陣営。</t>
+    <rPh sb="11" eb="12">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ジンエイ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="20" eb="24">
+      <t>ショウリジョウケン</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>オヨ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ノウリョク</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="40" eb="44">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ゼンメツ</t>
+    </rPh>
+    <rPh sb="53" eb="56">
+      <t>セイゾンシャ</t>
+    </rPh>
+    <rPh sb="57" eb="59">
+      <t>ハンスウ</t>
+    </rPh>
+    <rPh sb="59" eb="61">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="62" eb="63">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="64" eb="66">
+      <t>ジンエイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SidekickFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>curSidekick</t>
+  </si>
+  <si>
+    <t>現在のサイドキック</t>
+    <rPh sb="0" eb="2">
+      <t>ゲンザイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>curJackal</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>curLover</t>
+  </si>
+  <si>
+    <t>curSupportTarget</t>
+  </si>
+  <si>
+    <t>現在のサポート対象</t>
+    <rPh sb="0" eb="2">
+      <t>ゲンザイ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>タイショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>現在のジャッカル</t>
+    <rPh sb="0" eb="2">
+      <t>ゲンザイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>恋人</t>
+    <rPh sb="0" eb="2">
+      <t>コイビト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>playerName</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>roleName</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>役職</t>
+    <rPh sb="0" eb="2">
+      <t>ヤクショク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>プレイヤー名</t>
+    <rPh sb="5" eb="6">
+      <t>メイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -3133,10 +4323,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3418,10 +4611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q114"/>
+  <dimension ref="A1:Q117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A115" sqref="A115"/>
+    <sheetView tabSelected="1" topLeftCell="C100" workbookViewId="0">
+      <selection activeCell="M117" sqref="M117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -3800,10 +4993,10 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
+        <v>479</v>
+      </c>
+      <c r="M37" t="s">
         <v>480</v>
-      </c>
-      <c r="M37" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.4">
@@ -3811,7 +5004,7 @@
         <v>319</v>
       </c>
       <c r="M39" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.4">
@@ -3819,7 +5012,7 @@
         <v>321</v>
       </c>
       <c r="M40" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.4">
@@ -3827,7 +5020,7 @@
         <v>322</v>
       </c>
       <c r="M41" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.4">
@@ -3843,7 +5036,7 @@
         <v>320</v>
       </c>
       <c r="M44" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.4">
@@ -3851,7 +5044,7 @@
         <v>323</v>
       </c>
       <c r="M45" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.4">
@@ -3859,7 +5052,7 @@
         <v>325</v>
       </c>
       <c r="M46" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.4">
@@ -4174,18 +5367,18 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
+        <v>554</v>
+      </c>
+      <c r="M93" t="s">
         <v>555</v>
-      </c>
-      <c r="M93" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="M94" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.4">
@@ -4286,26 +5479,42 @@
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A112" t="s">
+        <v>557</v>
+      </c>
+      <c r="M112" t="s">
         <v>558</v>
-      </c>
-      <c r="M112" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A113" t="s">
+        <v>559</v>
+      </c>
+      <c r="M113" t="s">
         <v>560</v>
-      </c>
-      <c r="M113" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A114" t="s">
+        <v>561</v>
+      </c>
+      <c r="M114" t="s">
         <v>562</v>
       </c>
-      <c r="M114" t="s">
-        <v>563</v>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A116" t="s">
+        <v>610</v>
+      </c>
+      <c r="M116" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A117" t="s">
+        <v>611</v>
+      </c>
+      <c r="M117" t="s">
+        <v>612</v>
       </c>
     </row>
   </sheetData>
@@ -4317,16 +5526,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5C264A-D4F8-4177-9D21-7A3435066086}">
-  <dimension ref="A1:Q48"/>
+  <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
-    <col min="13" max="13" width="44.5" customWidth="1"/>
+    <col min="13" max="13" width="78.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.4">
@@ -4408,7 +5617,7 @@
         <v>105</v>
       </c>
       <c r="M5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.4">
@@ -4416,7 +5625,7 @@
         <v>106</v>
       </c>
       <c r="M6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.4">
@@ -4443,17 +5652,17 @@
         <v>225</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>424</v>
-      </c>
-      <c r="M11" t="s">
-        <v>438</v>
+    <row r="10" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>563</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="M12" t="s">
         <v>438</v>
@@ -4461,274 +5670,314 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="M13" t="s">
-        <v>110</v>
+        <v>438</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="M14" t="s">
-        <v>468</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="M15" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="M16" t="s">
-        <v>111</v>
+        <v>468</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="M17" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="M18" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="M19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="M20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="M21" t="s">
-        <v>439</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="M22" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="M23" t="s">
-        <v>465</v>
+        <v>440</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
+        <v>434</v>
+      </c>
+      <c r="M24" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
         <v>435</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M25" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:13" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>452</v>
-      </c>
-      <c r="M26" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A27" t="s">
-        <v>453</v>
-      </c>
-      <c r="M27" t="s">
-        <v>464</v>
+        <v>564</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>454</v>
+        <v>566</v>
       </c>
       <c r="M28" t="s">
-        <v>110</v>
+        <v>463</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="M29" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="M30" t="s">
-        <v>469</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
+        <v>454</v>
+      </c>
+      <c r="M31" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>455</v>
+      </c>
+      <c r="M32" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>456</v>
+      </c>
+      <c r="M33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A34" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="M31" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A32" s="1" t="s">
+      <c r="M34" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A35" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="M32" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A33" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="M33" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
-        <v>460</v>
-      </c>
-      <c r="M34" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
+      <c r="M35" t="s">
         <v>461</v>
-      </c>
-      <c r="M35" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>478</v>
+        <v>459</v>
       </c>
       <c r="M36" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.4">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
+        <v>460</v>
+      </c>
+      <c r="M37" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>537</v>
-      </c>
-      <c r="M38" t="s">
-        <v>538</v>
+        <v>567</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>539</v>
+        <v>477</v>
       </c>
       <c r="M39" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A40" t="s">
-        <v>540</v>
-      </c>
-      <c r="M40" t="s">
-        <v>110</v>
+        <v>478</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="M41" t="s">
-        <v>468</v>
+        <v>537</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="M42" t="s">
-        <v>469</v>
+        <v>537</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
+        <v>539</v>
+      </c>
+      <c r="M43" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
+        <v>540</v>
+      </c>
+      <c r="M44" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
+        <v>541</v>
+      </c>
+      <c r="M45" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
+        <v>542</v>
+      </c>
+      <c r="M46" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A47" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="M47" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A48" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="M48" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A49" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="M49" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
         <v>543</v>
       </c>
-      <c r="M43" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A44" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="M44" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A45" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="M45" t="s">
+      <c r="M50" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A46" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="M46" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A47" t="s">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A51" t="s">
         <v>544</v>
       </c>
-      <c r="M47" t="s">
+      <c r="M51" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A48" t="s">
-        <v>545</v>
-      </c>
-      <c r="M48" t="s">
-        <v>553</v>
+    <row r="52" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A52" t="s">
+        <v>570</v>
+      </c>
+      <c r="M52" s="2" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A53" t="s">
+        <v>581</v>
+      </c>
+      <c r="M53" s="2" t="s">
+        <v>582</v>
       </c>
     </row>
   </sheetData>
@@ -4740,16 +5989,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131ED9DB-7094-4FCA-8832-3F1005AB8270}">
-  <dimension ref="A1:Q53"/>
+  <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
-    <col min="13" max="13" width="43.875" customWidth="1"/>
+    <col min="13" max="13" width="65" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.4">
@@ -4831,7 +6080,7 @@
         <v>114</v>
       </c>
       <c r="M5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.4">
@@ -4839,7 +6088,7 @@
         <v>115</v>
       </c>
       <c r="M6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.4">
@@ -4898,17 +6147,17 @@
         <v>230</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
+    <row r="14" spans="1:17" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>572</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
         <v>382</v>
-      </c>
-      <c r="M15" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A16" s="1" t="s">
-        <v>381</v>
       </c>
       <c r="M16" t="s">
         <v>383</v>
@@ -4916,290 +6165,314 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
-        <v>368</v>
+        <v>381</v>
       </c>
       <c r="M17" t="s">
-        <v>110</v>
+        <v>383</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="M18" t="s">
-        <v>468</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="M19" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="M20" t="s">
-        <v>111</v>
+        <v>468</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="M21" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M22" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="M23" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="M24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="M25" t="s">
-        <v>384</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
       <c r="M26" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="M27" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
-        <v>400</v>
+        <v>377</v>
       </c>
       <c r="M28" t="s">
-        <v>402</v>
+        <v>386</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="M29" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
-        <v>378</v>
+        <v>401</v>
       </c>
       <c r="M30" t="s">
-        <v>390</v>
+        <v>403</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="M31" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="M32" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A33" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="M32" t="s">
+      <c r="M33" t="s">
         <v>389</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A33" t="s">
-        <v>391</v>
-      </c>
-      <c r="M33" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="M34" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
+        <v>392</v>
+      </c>
+      <c r="M35" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="64.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
+        <v>574</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
         <v>398</v>
       </c>
-      <c r="M35" t="s">
+      <c r="M37" t="s">
         <v>395</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A36" t="s">
-        <v>396</v>
-      </c>
-      <c r="M36" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>488</v>
+        <v>396</v>
       </c>
       <c r="M38" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A39" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="M39" t="s">
-        <v>498</v>
+        <v>397</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A40" s="1" t="s">
-        <v>490</v>
+      <c r="A40" t="s">
+        <v>487</v>
       </c>
       <c r="M40" t="s">
-        <v>110</v>
+        <v>497</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="M41" t="s">
-        <v>468</v>
+        <v>497</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="M42" t="s">
-        <v>469</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="M43" t="s">
-        <v>111</v>
+        <v>467</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="M44" t="s">
-        <v>123</v>
+        <v>468</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="M45" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A46" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="M46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="M47" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="M48" t="s">
-        <v>507</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="M49" t="s">
-        <v>506</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="M50" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A51" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="M51" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A52" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="M52" t="s">
         <v>509</v>
-      </c>
-      <c r="M50" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A51" t="s">
-        <v>501</v>
-      </c>
-      <c r="M51" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A52" t="s">
-        <v>502</v>
-      </c>
-      <c r="M52" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
+        <v>500</v>
+      </c>
+      <c r="M53" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A54" t="s">
+        <v>501</v>
+      </c>
+      <c r="M54" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A55" t="s">
+        <v>575</v>
+      </c>
+      <c r="M55" s="2" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A56" t="s">
+        <v>502</v>
+      </c>
+      <c r="M56" t="s">
         <v>503</v>
-      </c>
-      <c r="M53" t="s">
-        <v>504</v>
       </c>
     </row>
   </sheetData>
@@ -5211,16 +6484,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445F46B3-1A86-46EF-9440-E5378C8C2CDD}">
-  <dimension ref="A1:Q49"/>
+  <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView topLeftCell="B43" workbookViewId="0">
+      <selection activeCell="M52" sqref="M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="13" max="13" width="62.25" customWidth="1"/>
+    <col min="13" max="13" width="66" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.4">
@@ -5302,7 +6575,7 @@
         <v>128</v>
       </c>
       <c r="M5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.4">
@@ -5310,7 +6583,7 @@
         <v>129</v>
       </c>
       <c r="M6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.4">
@@ -5409,164 +6682,164 @@
         <v>234</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:13" ht="120.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
+        <v>578</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
         <v>362</v>
       </c>
-      <c r="M19" t="s">
+      <c r="M20" t="s">
         <v>363</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
-        <v>257</v>
-      </c>
-      <c r="M21" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>534</v>
+        <v>257</v>
       </c>
       <c r="M22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>138</v>
+        <v>533</v>
       </c>
       <c r="M23" t="s">
-        <v>168</v>
+        <v>259</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M24" t="s">
-        <v>110</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M25" t="s">
-        <v>470</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M26" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M27" t="s">
-        <v>164</v>
+        <v>470</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M28" t="s">
-        <v>123</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M29" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M30" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>342</v>
+        <v>146</v>
       </c>
       <c r="M32" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
+        <v>342</v>
+      </c>
+      <c r="M33" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
         <v>148</v>
       </c>
-      <c r="M33" t="s">
+      <c r="M34" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A35" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="M34" t="s">
+      <c r="M35" t="s">
         <v>315</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
-        <v>150</v>
-      </c>
-      <c r="M35" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M36" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M37" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="M38" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>533</v>
+        <v>154</v>
       </c>
       <c r="M39" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.4">
@@ -5574,79 +6847,119 @@
         <v>532</v>
       </c>
       <c r="M40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>316</v>
+        <v>531</v>
       </c>
       <c r="M41" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
+        <v>316</v>
+      </c>
+      <c r="M42" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
         <v>161</v>
       </c>
-      <c r="M42" t="s">
+      <c r="M43" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A44" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="M43" t="s">
+      <c r="M44" t="s">
         <v>318</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A44" t="s">
-        <v>163</v>
-      </c>
-      <c r="M44" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="M45" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M46" t="s">
-        <v>165</v>
+        <v>472</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>235</v>
+        <v>167</v>
       </c>
       <c r="M47" t="s">
-        <v>240</v>
+        <v>165</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M48" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
+        <v>236</v>
+      </c>
+      <c r="M49" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="105" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
+        <v>579</v>
+      </c>
+      <c r="M50" s="2" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A51" t="s">
+        <v>602</v>
+      </c>
+      <c r="M51" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A52" t="s">
         <v>237</v>
       </c>
-      <c r="M49" t="s">
+      <c r="M52" t="s">
         <v>238</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A53" t="s">
+        <v>601</v>
+      </c>
+      <c r="M53" s="2" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A54" t="s">
+        <v>604</v>
+      </c>
+      <c r="M54" t="s">
+        <v>608</v>
       </c>
     </row>
   </sheetData>
@@ -5658,16 +6971,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA3747E3-550F-4585-A066-931F491B69D2}">
-  <dimension ref="A1:Q68"/>
+  <dimension ref="A1:Q78"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView topLeftCell="D55" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="38.375" customWidth="1"/>
-    <col min="13" max="13" width="74.625" customWidth="1"/>
+    <col min="13" max="13" width="86.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.4">
@@ -5765,7 +7078,7 @@
         <v>173</v>
       </c>
       <c r="M7" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.4">
@@ -5773,7 +7086,7 @@
         <v>175</v>
       </c>
       <c r="M8" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.4">
@@ -5837,7 +7150,7 @@
         <v>190</v>
       </c>
       <c r="M16" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.4">
@@ -5845,7 +7158,7 @@
         <v>191</v>
       </c>
       <c r="M17" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.4">
@@ -5904,340 +7217,420 @@
         <v>243</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:13" ht="75" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>244</v>
-      </c>
-      <c r="M25" t="s">
-        <v>247</v>
+        <v>584</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>587</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="M26" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>347</v>
+        <v>245</v>
       </c>
       <c r="M27" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="187.5" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>350</v>
-      </c>
-      <c r="M28" t="s">
-        <v>351</v>
+        <v>585</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>586</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="M29" t="s">
-        <v>352</v>
+        <v>348</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>350</v>
+      </c>
+      <c r="M30" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>264</v>
+        <v>349</v>
       </c>
       <c r="M31" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
-        <v>200</v>
-      </c>
-      <c r="M32" t="s">
-        <v>203</v>
+        <v>352</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>201</v>
+        <v>264</v>
       </c>
       <c r="M33" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="M34" t="s">
-        <v>170</v>
+        <v>203</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="M35" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="M36" t="s">
-        <v>209</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M37" t="s">
-        <v>174</v>
+        <v>208</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="M38" t="s">
-        <v>468</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M39" t="s">
-        <v>469</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M40" t="s">
-        <v>111</v>
+        <v>467</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="M41" t="s">
-        <v>214</v>
+        <v>468</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="M42" t="s">
-        <v>216</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="M43" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="M44" t="s">
-        <v>123</v>
+        <v>216</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="M45" t="s">
-        <v>122</v>
+        <v>222</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="M46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="M47" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>248</v>
+        <v>220</v>
       </c>
       <c r="M48" t="s">
-        <v>253</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>249</v>
+        <v>221</v>
       </c>
       <c r="M49" t="s">
-        <v>250</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>535</v>
+        <v>248</v>
       </c>
       <c r="M50" t="s">
-        <v>536</v>
+        <v>253</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>404</v>
+        <v>249</v>
       </c>
       <c r="M51" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.4">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="98.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A52" t="s">
+        <v>588</v>
+      </c>
+      <c r="M52" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="116.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
-        <v>511</v>
-      </c>
-      <c r="M53" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.4">
+        <v>590</v>
+      </c>
+      <c r="M53" s="2" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="93.75" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
-        <v>513</v>
-      </c>
-      <c r="M54" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.4">
+        <v>589</v>
+      </c>
+      <c r="M54" s="2" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
-        <v>514</v>
-      </c>
-      <c r="M55" t="s">
-        <v>515</v>
+        <v>594</v>
+      </c>
+      <c r="M55" s="2" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
-        <v>517</v>
+        <v>534</v>
       </c>
       <c r="M56" t="s">
-        <v>512</v>
+        <v>535</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
-        <v>518</v>
-      </c>
-      <c r="M57" t="s">
-        <v>170</v>
+        <v>605</v>
+      </c>
+      <c r="M57" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
-        <v>519</v>
+        <v>404</v>
       </c>
       <c r="M58" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A59" t="s">
-        <v>520</v>
-      </c>
-      <c r="M59" t="s">
-        <v>209</v>
+        <v>405</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
-        <v>521</v>
+        <v>510</v>
       </c>
       <c r="M60" t="s">
-        <v>468</v>
+        <v>511</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
-        <v>522</v>
+        <v>512</v>
       </c>
       <c r="M61" t="s">
-        <v>469</v>
+        <v>515</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
-        <v>523</v>
+        <v>513</v>
       </c>
       <c r="M62" t="s">
-        <v>111</v>
+        <v>514</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="M63" t="s">
-        <v>123</v>
+        <v>511</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="M64" t="s">
-        <v>122</v>
+        <v>170</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="M65" t="s">
-        <v>124</v>
+        <v>208</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="M66" t="s">
-        <v>125</v>
+        <v>209</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="M67" t="s">
-        <v>530</v>
+        <v>467</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
+        <v>521</v>
+      </c>
+      <c r="M68" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A69" t="s">
+        <v>522</v>
+      </c>
+      <c r="M69" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A70" t="s">
+        <v>523</v>
+      </c>
+      <c r="M70" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A71" t="s">
+        <v>524</v>
+      </c>
+      <c r="M71" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A72" t="s">
+        <v>525</v>
+      </c>
+      <c r="M72" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A73" t="s">
+        <v>526</v>
+      </c>
+      <c r="M73" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A74" t="s">
+        <v>527</v>
+      </c>
+      <c r="M74" t="s">
         <v>529</v>
       </c>
-      <c r="M68" t="s">
-        <v>531</v>
+    </row>
+    <row r="75" spans="1:13" ht="81" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A75" t="s">
+        <v>528</v>
+      </c>
+      <c r="M75" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="75" x14ac:dyDescent="0.4">
+      <c r="A76" t="s">
+        <v>596</v>
+      </c>
+      <c r="M76" s="2" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" ht="75" x14ac:dyDescent="0.4">
+      <c r="A77" t="s">
+        <v>598</v>
+      </c>
+      <c r="M77" s="2" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A78" t="s">
+        <v>606</v>
+      </c>
+      <c r="M78" t="s">
+        <v>607</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat:vanila role full desc
</commit_message>
<xml_diff>
--- a/transData.xlsx
+++ b/transData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ドキュメント\VisualStudioProject\AmongUs\ExtremeRoles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE939211-5999-41D0-B98F-63F857D69FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC5F7B2-016A-4986-ABFC-83F3ACD15E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13740" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="624">
   <si>
     <t>English</t>
   </si>
@@ -3095,38 +3095,6 @@
   </si>
   <si>
     <t>SheriffFullDescription</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>キルが可能なクルー役職。ただし、キル可能回数には上限がある
-キルを行おうとした相手がクルー役職であればキルは失敗して死亡する</t>
-    <rPh sb="3" eb="5">
-      <t>カノウ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>カノウ</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>カイスウ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>ジョウゲン</t>
-    </rPh>
-    <rPh sb="33" eb="34">
-      <t>オコナ</t>
-    </rPh>
-    <rPh sb="39" eb="41">
-      <t>アイテ</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>ヤクショク</t>
-    </rPh>
-    <rPh sb="54" eb="56">
-      <t>シッパイ</t>
-    </rPh>
-    <rPh sb="58" eb="60">
-      <t>シボウ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -3167,54 +3135,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>緊急修理が行えるクルー役職
-緊急修理は緊急タスク(サボタージ)発生時、使用可能
-緊急修理が発動すると緊急タスクはすぐに完了し、マップ内のドアが全て開きます</t>
-    <rPh sb="0" eb="2">
-      <t>キンキュウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>シュウリ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>オコナ</t>
-    </rPh>
-    <rPh sb="14" eb="18">
-      <t>キンキュウ</t>
-    </rPh>
-    <rPh sb="19" eb="21">
-      <t>キンキュウ</t>
-    </rPh>
-    <rPh sb="31" eb="34">
-      <t>ハッセイジ</t>
-    </rPh>
-    <rPh sb="35" eb="39">
-      <t>シヨウカノウ</t>
-    </rPh>
-    <rPh sb="40" eb="44">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>ハツドウ</t>
-    </rPh>
-    <rPh sb="50" eb="52">
-      <t>キンキュウ</t>
-    </rPh>
-    <rPh sb="59" eb="61">
-      <t>カンリョウ</t>
-    </rPh>
-    <rPh sb="66" eb="67">
-      <t>ナイ</t>
-    </rPh>
-    <rPh sb="71" eb="72">
-      <t>スベ</t>
-    </rPh>
-    <rPh sb="73" eb="74">
-      <t>ヒラ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>NeetFullDescription</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -3246,35 +3166,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Extreme Rolesの各役職の共通設定が適用できるインポスター役職
-設定内容は以下を確認</t>
-    <rPh sb="14" eb="17">
-      <t>カクヤクショク</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>キョウツウ</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>テキヨウ</t>
-    </rPh>
-    <rPh sb="34" eb="36">
-      <t>ヤクショク</t>
-    </rPh>
-    <rPh sb="37" eb="41">
-      <t>セッテイナイヨウ</t>
-    </rPh>
-    <rPh sb="42" eb="44">
-      <t>イカ</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>カクニン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>EvolverFullDescription</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -3311,51 +3202,6 @@
     </rPh>
     <rPh sb="43" eb="44">
       <t>オ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>死体を喰うことで、キルクールタイムが短くなるインポスター役職
-捕食中は死体の近くに居なければならない
-捕食後は新しいキルクールタイムが適用される</t>
-    <rPh sb="0" eb="2">
-      <t>シタイ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>ク</t>
-    </rPh>
-    <rPh sb="18" eb="19">
-      <t>ミジカ</t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t>ヤクショク</t>
-    </rPh>
-    <rPh sb="31" eb="33">
-      <t>ホショク</t>
-    </rPh>
-    <rPh sb="33" eb="34">
-      <t>チュウ</t>
-    </rPh>
-    <rPh sb="35" eb="37">
-      <t>シタイ</t>
-    </rPh>
-    <rPh sb="38" eb="39">
-      <t>チカ</t>
-    </rPh>
-    <rPh sb="41" eb="42">
-      <t>イ</t>
-    </rPh>
-    <rPh sb="51" eb="53">
-      <t>ホショク</t>
-    </rPh>
-    <rPh sb="53" eb="54">
-      <t>ゴ</t>
-    </rPh>
-    <rPh sb="55" eb="56">
-      <t>アタラ</t>
-    </rPh>
-    <rPh sb="67" eb="69">
-      <t>テキヨウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -3494,226 +3340,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>インポスター陣営に新しい勝利条件を追加するインポスター役職
-新しい勝利条件：アサシンの特殊能力でマーリンを当てる
-アサシンの特殊能力：マーリン指定の特殊会議
-マーリン指定の特殊会議：全員が参加するが能力を発動させたアサシン以外投票不可
-　　　　　　　　　　　　スキップ不可、チャット不可、死亡している人にも投票可
-　　　　　　　　　　　　投票先がマーリンであればインポスター勝利、それ以外の
-　　　　　　　　　　　　場合、ゲームが続行(マーリンの能力は継続)
-特殊能力発動条件：追放された場合、自身がキルされた場合の処理は設定可
-上記の能力以外は普通のインポスターのため、マーリンを探りつつ潜伏しキルを行う必要がある</t>
-    <rPh sb="6" eb="8">
-      <t>ジンエイ</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>アタラ</t>
-    </rPh>
-    <rPh sb="12" eb="16">
-      <t>ショウリジョウケン</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ツイカ</t>
-    </rPh>
-    <rPh sb="27" eb="29">
-      <t>ヤクショク</t>
-    </rPh>
-    <rPh sb="30" eb="31">
-      <t>アタラ</t>
-    </rPh>
-    <rPh sb="43" eb="47">
-      <t>トクシュノウリョク</t>
-    </rPh>
-    <rPh sb="53" eb="54">
-      <t>ア</t>
-    </rPh>
-    <rPh sb="62" eb="66">
-      <t>トク</t>
-    </rPh>
-    <rPh sb="71" eb="73">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="74" eb="76">
-      <t>トクシュ</t>
-    </rPh>
-    <rPh sb="76" eb="78">
-      <t>カイギ</t>
-    </rPh>
-    <rPh sb="83" eb="85">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="86" eb="88">
-      <t>トクシュ</t>
-    </rPh>
-    <rPh sb="88" eb="90">
-      <t>カイギ</t>
-    </rPh>
-    <rPh sb="91" eb="93">
-      <t>ゼンイン</t>
-    </rPh>
-    <rPh sb="94" eb="96">
-      <t>サンカ</t>
-    </rPh>
-    <rPh sb="99" eb="101">
-      <t>ノウリョク</t>
-    </rPh>
-    <rPh sb="102" eb="104">
-      <t>ハツドウ</t>
-    </rPh>
-    <rPh sb="111" eb="113">
-      <t>イガイ</t>
-    </rPh>
-    <rPh sb="113" eb="115">
-      <t>トウヒョウ</t>
-    </rPh>
-    <rPh sb="115" eb="117">
-      <t>フカ</t>
-    </rPh>
-    <rPh sb="134" eb="136">
-      <t>フカ</t>
-    </rPh>
-    <rPh sb="141" eb="143">
-      <t>フカ</t>
-    </rPh>
-    <rPh sb="144" eb="146">
-      <t>シボウ</t>
-    </rPh>
-    <rPh sb="150" eb="151">
-      <t>ヒト</t>
-    </rPh>
-    <rPh sb="153" eb="155">
-      <t>トウヒョウ</t>
-    </rPh>
-    <rPh sb="155" eb="156">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="169" eb="171">
-      <t>トウヒョウ</t>
-    </rPh>
-    <rPh sb="171" eb="172">
-      <t>サキ</t>
-    </rPh>
-    <rPh sb="187" eb="189">
-      <t>ショウリ</t>
-    </rPh>
-    <rPh sb="192" eb="194">
-      <t>イガイ</t>
-    </rPh>
-    <rPh sb="208" eb="210">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="215" eb="217">
-      <t>ゾッコウ</t>
-    </rPh>
-    <rPh sb="223" eb="225">
-      <t>ノウリョク</t>
-    </rPh>
-    <rPh sb="226" eb="228">
-      <t>ケイゾク</t>
-    </rPh>
-    <rPh sb="230" eb="234">
-      <t>トクシュ</t>
-    </rPh>
-    <rPh sb="234" eb="238">
-      <t>ハツドウジョウケン</t>
-    </rPh>
-    <rPh sb="239" eb="241">
-      <t>ツイホウ</t>
-    </rPh>
-    <rPh sb="244" eb="246">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="255" eb="257">
-      <t>バアイショリ</t>
-    </rPh>
-    <rPh sb="265" eb="267">
-      <t>ジョウキ</t>
-    </rPh>
-    <rPh sb="268" eb="270">
-      <t>ノウリョク</t>
-    </rPh>
-    <rPh sb="270" eb="272">
-      <t>イガイ</t>
-    </rPh>
-    <rPh sb="273" eb="275">
-      <t>フツウ</t>
-    </rPh>
-    <rPh sb="291" eb="292">
-      <t>サグ</t>
-    </rPh>
-    <rPh sb="295" eb="297">
-      <t>センプク</t>
-    </rPh>
-    <rPh sb="301" eb="302">
-      <t>オコナ</t>
-    </rPh>
-    <rPh sb="303" eb="305">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>インポスターが誰か分かるクルー役職
-アサシンの特殊能力によって指定された場合、クルー全体の敗北
-インポスターが分かるので会議を主導しつつ、身を隠す必要がある
-インポスターに近い設定の役職のため、注意が必要</t>
-    <rPh sb="7" eb="8">
-      <t>ダレ</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>ワ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>ヤクショク</t>
-    </rPh>
-    <rPh sb="23" eb="27">
-      <t>トクシュノウリョク</t>
-    </rPh>
-    <rPh sb="31" eb="33">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="42" eb="44">
-      <t>ゼンタイ</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>ハイボク</t>
-    </rPh>
-    <rPh sb="55" eb="56">
-      <t>ワ</t>
-    </rPh>
-    <rPh sb="60" eb="62">
-      <t>カイギ</t>
-    </rPh>
-    <rPh sb="63" eb="65">
-      <t>シュドウ</t>
-    </rPh>
-    <rPh sb="69" eb="70">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="71" eb="72">
-      <t>カク</t>
-    </rPh>
-    <rPh sb="73" eb="75">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <rPh sb="86" eb="87">
-      <t>チカ</t>
-    </rPh>
-    <rPh sb="88" eb="90">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="91" eb="93">
-      <t>ヤクショク</t>
-    </rPh>
-    <rPh sb="97" eb="99">
-      <t>チュウイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>LoverFullDescription</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -3766,149 +3392,6 @@
     </rPh>
     <rPh sb="50" eb="52">
       <t>シュウリョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>複数人1組のインポスター役職
-勝利条件1：インポスター勝利、ただし、同じ組は敗北
-勝利条件2：同じ組のタスクが全て終了すること
-勝利条件3：生存者が同じ組以下になること
-同じ組の人が一定数以下になると自決もしくは第三陣営に変化する
-自決を行う人数は設定により変化する</t>
-    <rPh sb="0" eb="3">
-      <t>フクスウニン</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>クミ</t>
-    </rPh>
-    <rPh sb="15" eb="19">
-      <t>ショウリジョウケン</t>
-    </rPh>
-    <rPh sb="27" eb="29">
-      <t>ショウリ</t>
-    </rPh>
-    <rPh sb="34" eb="35">
-      <t>オナ</t>
-    </rPh>
-    <rPh sb="38" eb="40">
-      <t>ハイボク</t>
-    </rPh>
-    <rPh sb="41" eb="45">
-      <t>ショウリ</t>
-    </rPh>
-    <rPh sb="64" eb="68">
-      <t>ショウリ</t>
-    </rPh>
-    <rPh sb="85" eb="86">
-      <t>オナ</t>
-    </rPh>
-    <rPh sb="87" eb="88">
-      <t>クミ</t>
-    </rPh>
-    <rPh sb="89" eb="90">
-      <t>ヒト</t>
-    </rPh>
-    <rPh sb="91" eb="94">
-      <t>イッテイスウ</t>
-    </rPh>
-    <rPh sb="94" eb="96">
-      <t>イカ</t>
-    </rPh>
-    <rPh sb="100" eb="102">
-      <t>ジケツ</t>
-    </rPh>
-    <rPh sb="106" eb="110">
-      <t>ダイ</t>
-    </rPh>
-    <rPh sb="111" eb="113">
-      <t>ヘンカ</t>
-    </rPh>
-    <rPh sb="116" eb="118">
-      <t>ジケツ</t>
-    </rPh>
-    <rPh sb="119" eb="120">
-      <t>オコナ</t>
-    </rPh>
-    <rPh sb="121" eb="123">
-      <t>ニンズウ</t>
-    </rPh>
-    <rPh sb="124" eb="126">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="129" eb="131">
-      <t>ヘンカ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>複数人1組のクルー役職
-勝利条件1：クルー勝利、ただし、同じ組で別陣営の人が居た場合その人は敗北
-勝利条件2：生存者が同じ組以下になること
-同じ組の人が一定数以下になると自決もしくは第三陣営に変化する
-自決を行う人数は設定により変化する</t>
-    <rPh sb="0" eb="3">
-      <t>フクスウニン</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>クミ</t>
-    </rPh>
-    <rPh sb="32" eb="33">
-      <t>ベツ</t>
-    </rPh>
-    <rPh sb="33" eb="35">
-      <t>ジンエイ</t>
-    </rPh>
-    <rPh sb="36" eb="37">
-      <t>ヒト</t>
-    </rPh>
-    <rPh sb="38" eb="39">
-      <t>イ</t>
-    </rPh>
-    <rPh sb="40" eb="42">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="44" eb="45">
-      <t>ヒト</t>
-    </rPh>
-    <rPh sb="70" eb="71">
-      <t>オナ</t>
-    </rPh>
-    <rPh sb="72" eb="73">
-      <t>クミ</t>
-    </rPh>
-    <rPh sb="74" eb="75">
-      <t>ヒト</t>
-    </rPh>
-    <rPh sb="76" eb="79">
-      <t>イッテイスウ</t>
-    </rPh>
-    <rPh sb="79" eb="81">
-      <t>イカ</t>
-    </rPh>
-    <rPh sb="85" eb="87">
-      <t>ジケツ</t>
-    </rPh>
-    <rPh sb="91" eb="95">
-      <t>ダイ</t>
-    </rPh>
-    <rPh sb="96" eb="98">
-      <t>ヘンカ</t>
-    </rPh>
-    <rPh sb="101" eb="103">
-      <t>ジケツ</t>
-    </rPh>
-    <rPh sb="104" eb="105">
-      <t>オコナ</t>
-    </rPh>
-    <rPh sb="106" eb="108">
-      <t>ニンズウ</t>
-    </rPh>
-    <rPh sb="109" eb="111">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="114" eb="116">
-      <t>ヘンカ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -4294,6 +3777,659 @@
     </rPh>
     <rPh sb="64" eb="66">
       <t>ジンエイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>複数人1組のクルー役職
+勝利条件1：クルー勝利、ただし、同じ組で別陣営の人が居た場合
+その人は敗北
+勝利条件2：生存者が同じ組以下になること
+同じ組の人が一定数以下になると自決もしくは第三陣営に
+変化する
+自決を行う人数は設定により変化する</t>
+    <rPh sb="0" eb="3">
+      <t>フクスウニン</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>クミ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>ベツ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ジンエイ</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="71" eb="72">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="73" eb="74">
+      <t>クミ</t>
+    </rPh>
+    <rPh sb="75" eb="76">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="77" eb="80">
+      <t>イッテイスウ</t>
+    </rPh>
+    <rPh sb="80" eb="82">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="86" eb="88">
+      <t>ジケツ</t>
+    </rPh>
+    <rPh sb="92" eb="96">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="98" eb="100">
+      <t>ヘンカ</t>
+    </rPh>
+    <rPh sb="103" eb="105">
+      <t>ジケツ</t>
+    </rPh>
+    <rPh sb="106" eb="107">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="108" eb="110">
+      <t>ニンズウ</t>
+    </rPh>
+    <rPh sb="111" eb="113">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="116" eb="118">
+      <t>ヘンカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>複数人1組のインポスター役職
+勝利条件1：インポスター勝利、ただし、同じ組は敗北
+勝利条件2：同じ組のタスクが全て終了すること
+勝利条件3：生存者が同じ組以下になること
+同じ組の人が一定数以下になると自決もしくは第三陣営に
+変化する
+自決を行う人数は設定により変化する</t>
+    <rPh sb="0" eb="3">
+      <t>フクスウニン</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>クミ</t>
+    </rPh>
+    <rPh sb="15" eb="19">
+      <t>ショウリジョウケン</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ショウリ</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>ハイボク</t>
+    </rPh>
+    <rPh sb="41" eb="45">
+      <t>ショウリ</t>
+    </rPh>
+    <rPh sb="64" eb="68">
+      <t>ショウリ</t>
+    </rPh>
+    <rPh sb="85" eb="86">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="87" eb="88">
+      <t>クミ</t>
+    </rPh>
+    <rPh sb="89" eb="90">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="91" eb="94">
+      <t>イッテイスウ</t>
+    </rPh>
+    <rPh sb="94" eb="96">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="100" eb="102">
+      <t>ジケツ</t>
+    </rPh>
+    <rPh sb="106" eb="110">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="112" eb="114">
+      <t>ヘンカ</t>
+    </rPh>
+    <rPh sb="117" eb="119">
+      <t>ジケツ</t>
+    </rPh>
+    <rPh sb="120" eb="121">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="122" eb="124">
+      <t>ニンズウ</t>
+    </rPh>
+    <rPh sb="125" eb="127">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="130" eb="132">
+      <t>ヘンカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>インポスターが誰か分かるクルー役職
+アサシンの特殊能力によって指定された場合、クルー全体の敗北
+インポスターが分かるので会議を主導しつつ身を隠す必要がある
+インポスターに近い設定の役職のため、注意が必要</t>
+    <rPh sb="7" eb="8">
+      <t>ダレ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>ワ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="23" eb="27">
+      <t>トクシュノウリョク</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>ゼンタイ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ハイボク</t>
+    </rPh>
+    <rPh sb="55" eb="56">
+      <t>ワ</t>
+    </rPh>
+    <rPh sb="60" eb="62">
+      <t>カイギ</t>
+    </rPh>
+    <rPh sb="63" eb="65">
+      <t>シュドウ</t>
+    </rPh>
+    <rPh sb="68" eb="69">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="70" eb="71">
+      <t>カク</t>
+    </rPh>
+    <rPh sb="72" eb="74">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="85" eb="86">
+      <t>チカ</t>
+    </rPh>
+    <rPh sb="87" eb="89">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="90" eb="92">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="96" eb="98">
+      <t>チュウイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>インポスター陣営に新しい勝利条件を追加するインポスター役職
+新しい勝利条件：アサシンの特殊能力でマーリンを当てる
+アサシンの特殊能力：マーリン指定の特殊会議
+マーリン指定の特殊会議：
+　全員が参加するが能力を発動させたアサシン以外投票不可
+　スキップ不可、チャット不可、死亡している人にも投票可
+　投票先がマーリンであればインポスター勝利、それ以外の
+　場合、ゲームが続行(マーリンの能力は継続)
+特殊能力発動条件：追放された場合、自身がキルされた場合の
+処理は設定可
+上記の能力以外は普通のインポスターのため、マーリンを
+探りつつ潜伏しキルを行う必要がある</t>
+    <rPh sb="6" eb="8">
+      <t>ジンエイ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>アタラ</t>
+    </rPh>
+    <rPh sb="12" eb="16">
+      <t>ショウリジョウケン</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ツイカ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>アタラ</t>
+    </rPh>
+    <rPh sb="43" eb="47">
+      <t>トクシュノウリョク</t>
+    </rPh>
+    <rPh sb="53" eb="54">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="62" eb="66">
+      <t>トク</t>
+    </rPh>
+    <rPh sb="71" eb="73">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="74" eb="76">
+      <t>トクシュ</t>
+    </rPh>
+    <rPh sb="76" eb="78">
+      <t>カイギ</t>
+    </rPh>
+    <rPh sb="83" eb="85">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="86" eb="88">
+      <t>トクシュ</t>
+    </rPh>
+    <rPh sb="88" eb="90">
+      <t>カイギ</t>
+    </rPh>
+    <rPh sb="93" eb="95">
+      <t>ゼンイン</t>
+    </rPh>
+    <rPh sb="96" eb="98">
+      <t>サンカ</t>
+    </rPh>
+    <rPh sb="101" eb="103">
+      <t>ノウリョク</t>
+    </rPh>
+    <rPh sb="104" eb="106">
+      <t>ハツドウ</t>
+    </rPh>
+    <rPh sb="113" eb="115">
+      <t>イガイ</t>
+    </rPh>
+    <rPh sb="115" eb="117">
+      <t>トウヒョウ</t>
+    </rPh>
+    <rPh sb="117" eb="119">
+      <t>フカ</t>
+    </rPh>
+    <rPh sb="125" eb="127">
+      <t>フカ</t>
+    </rPh>
+    <rPh sb="132" eb="134">
+      <t>フカ</t>
+    </rPh>
+    <rPh sb="135" eb="137">
+      <t>シボウ</t>
+    </rPh>
+    <rPh sb="141" eb="142">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="144" eb="146">
+      <t>トウヒョウ</t>
+    </rPh>
+    <rPh sb="146" eb="147">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="149" eb="151">
+      <t>トウヒョウ</t>
+    </rPh>
+    <rPh sb="151" eb="152">
+      <t>サキ</t>
+    </rPh>
+    <rPh sb="167" eb="169">
+      <t>ショウリ</t>
+    </rPh>
+    <rPh sb="172" eb="174">
+      <t>イガイ</t>
+    </rPh>
+    <rPh sb="177" eb="179">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="184" eb="186">
+      <t>ゾッコウ</t>
+    </rPh>
+    <rPh sb="192" eb="194">
+      <t>ノウリョク</t>
+    </rPh>
+    <rPh sb="195" eb="197">
+      <t>ケイゾク</t>
+    </rPh>
+    <rPh sb="199" eb="203">
+      <t>トクシュ</t>
+    </rPh>
+    <rPh sb="203" eb="207">
+      <t>ハツドウジョウケン</t>
+    </rPh>
+    <rPh sb="208" eb="210">
+      <t>ツイホウ</t>
+    </rPh>
+    <rPh sb="213" eb="215">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="224" eb="226">
+      <t>バアイショリ</t>
+    </rPh>
+    <rPh sb="235" eb="237">
+      <t>ジョウキ</t>
+    </rPh>
+    <rPh sb="238" eb="240">
+      <t>ノウリョク</t>
+    </rPh>
+    <rPh sb="240" eb="242">
+      <t>イガイ</t>
+    </rPh>
+    <rPh sb="243" eb="245">
+      <t>フツウ</t>
+    </rPh>
+    <rPh sb="262" eb="263">
+      <t>サグ</t>
+    </rPh>
+    <rPh sb="266" eb="268">
+      <t>センプク</t>
+    </rPh>
+    <rPh sb="272" eb="273">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="274" eb="276">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>インポスター役職
+死体を捕食することで、キルクールタイムが短くなる
+捕食中は死体の近くに居なければならない
+捕食後は新しいキルクールタイムが適用される</t>
+    <rPh sb="9" eb="11">
+      <t>シタイ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ホショク</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>ミジカ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>ホショク</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>チュウ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>シタイ</t>
+    </rPh>
+    <rPh sb="41" eb="42">
+      <t>チカ</t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>ホショク</t>
+    </rPh>
+    <rPh sb="56" eb="57">
+      <t>ゴ</t>
+    </rPh>
+    <rPh sb="58" eb="59">
+      <t>アタラ</t>
+    </rPh>
+    <rPh sb="70" eb="72">
+      <t>テキヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>インポスター役職
+Extreme Rolesの各役職の共通設定が適用できる
+設定内容は以下を確認</t>
+    <rPh sb="23" eb="26">
+      <t>カクヤクショク</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>キョウツウ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>テキヨウ</t>
+    </rPh>
+    <rPh sb="38" eb="42">
+      <t>セッテイナイヨウ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>緊急修理が行えるクルー役職
+緊急修理は緊急タスク(サボタージ)発生時、使用可能
+緊急修理が発動すると緊急タスクはすぐに完了し、
+マップ内のドアが全て開きます</t>
+    <rPh sb="0" eb="2">
+      <t>キンキュウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>シュウリ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="14" eb="18">
+      <t>キンキュウ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>キンキュウ</t>
+    </rPh>
+    <rPh sb="31" eb="34">
+      <t>ハッセイジ</t>
+    </rPh>
+    <rPh sb="35" eb="39">
+      <t>シヨウカノウ</t>
+    </rPh>
+    <rPh sb="40" eb="44">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ハツドウ</t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t>キンキュウ</t>
+    </rPh>
+    <rPh sb="59" eb="61">
+      <t>カンリョウ</t>
+    </rPh>
+    <rPh sb="67" eb="68">
+      <t>ナイ</t>
+    </rPh>
+    <rPh sb="72" eb="73">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="74" eb="75">
+      <t>ヒラ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>キルが可能なクルー役職。ただし、キル可能回数には上限がある
+キルを行おうとした相手がクルー役職であればキルは失敗して
+自身が死亡する</t>
+    <rPh sb="3" eb="5">
+      <t>カノウ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>カノウ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>カイスウ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ジョウゲン</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>アイテ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>シッパイ</t>
+    </rPh>
+    <rPh sb="59" eb="61">
+      <t>ジシン</t>
+    </rPh>
+    <rPh sb="62" eb="64">
+      <t>シボウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CrewmateFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>EngineerFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ScientistFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>タスクを行うクルー役職</t>
+    <rPh sb="4" eb="5">
+      <t>オコナ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ベントが使えるクルー役職</t>
+    <rPh sb="4" eb="5">
+      <t>ツカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>どこでもバイタルが使えるクルー役職
+バイタルの使用時間は有限
+使用時間は時間経過かタスクを完了することで回復する</t>
+    <rPh sb="9" eb="10">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ジカン</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>ユウゲン</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ジカン</t>
+    </rPh>
+    <rPh sb="36" eb="40">
+      <t>ジカンケイカ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>カンリョウ</t>
+    </rPh>
+    <rPh sb="52" eb="54">
+      <t>カイフク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ImpostorFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>インポスター役職
+キルやサボタージを行える
+タスク偽造等でクルーのふりをしろ</t>
+    <rPh sb="18" eb="19">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ギゾウ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>トウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ShapeshifterFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>他人に変身できるインポスター役職
+返信できる相手はキルした相手でも可
+変身中はクルーに気付かれないようにする必要がある
+キルやサボタージを行える
+タスク偽造等でクルーのふりをしろ</t>
+    <rPh sb="0" eb="2">
+      <t>タニン</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ヘンシン</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ヘンシン</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>アイテ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>アイテ</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ヘンシン</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>チュウ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>キヅ</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="69" eb="70">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="76" eb="78">
+      <t>ギゾウ</t>
+    </rPh>
+    <rPh sb="78" eb="79">
+      <t>トウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -4628,8 +4764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q117"/>
   <sheetViews>
-    <sheetView topLeftCell="C100" workbookViewId="0">
-      <selection activeCell="M117" sqref="M117"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -5518,18 +5654,18 @@
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A116" t="s">
-        <v>606</v>
+        <v>598</v>
       </c>
       <c r="M116" t="s">
-        <v>609</v>
+        <v>601</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A117" t="s">
-        <v>607</v>
+        <v>599</v>
       </c>
       <c r="M117" t="s">
-        <v>608</v>
+        <v>600</v>
       </c>
     </row>
   </sheetData>
@@ -5541,16 +5677,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5C264A-D4F8-4177-9D21-7A3435066086}">
-  <dimension ref="A1:Q53"/>
+  <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
-    <col min="13" max="13" width="78.375" customWidth="1"/>
+    <col min="13" max="13" width="56.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.4">
@@ -5605,394 +5741,419 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>254</v>
+        <v>614</v>
       </c>
       <c r="M2" t="s">
-        <v>109</v>
+        <v>617</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>615</v>
       </c>
       <c r="M3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="57" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>104</v>
-      </c>
-      <c r="M4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>105</v>
-      </c>
-      <c r="M5" t="s">
-        <v>467</v>
-      </c>
-    </row>
+        <v>616</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="41.25" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>254</v>
       </c>
       <c r="M6" t="s">
-        <v>468</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="M7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>223</v>
+        <v>104</v>
       </c>
       <c r="M8" t="s">
-        <v>226</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>224</v>
+        <v>105</v>
       </c>
       <c r="M9" t="s">
-        <v>225</v>
+        <v>467</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>563</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>568</v>
+        <v>106</v>
+      </c>
+      <c r="M10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>107</v>
+      </c>
+      <c r="M11" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>424</v>
+        <v>223</v>
       </c>
       <c r="M12" t="s">
-        <v>438</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>425</v>
+        <v>224</v>
       </c>
       <c r="M13" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>426</v>
-      </c>
-      <c r="M14" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>427</v>
-      </c>
-      <c r="M15" t="s">
-        <v>467</v>
+        <v>563</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>567</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="M16" t="s">
-        <v>468</v>
+        <v>438</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="M17" t="s">
-        <v>111</v>
+        <v>438</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="M18" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="M19" t="s">
-        <v>122</v>
+        <v>467</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="M20" t="s">
-        <v>124</v>
+        <v>468</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="M21" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="M22" t="s">
-        <v>439</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="M23" t="s">
-        <v>440</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="M24" t="s">
-        <v>464</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="M25" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="37.5" x14ac:dyDescent="0.4">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>564</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>565</v>
+        <v>436</v>
+      </c>
+      <c r="M26" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>437</v>
+      </c>
+      <c r="M27" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>566</v>
+        <v>434</v>
       </c>
       <c r="M28" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>452</v>
+        <v>435</v>
       </c>
       <c r="M29" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.4">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>453</v>
-      </c>
-      <c r="M30" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
-        <v>454</v>
-      </c>
-      <c r="M31" t="s">
-        <v>467</v>
+        <v>564</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>613</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>455</v>
+        <v>565</v>
       </c>
       <c r="M32" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="M33" t="s">
-        <v>111</v>
+        <v>463</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A34" s="1" t="s">
-        <v>457</v>
+      <c r="A34" t="s">
+        <v>453</v>
       </c>
       <c r="M34" t="s">
-        <v>462</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A35" s="1" t="s">
-        <v>458</v>
+      <c r="A35" t="s">
+        <v>454</v>
       </c>
       <c r="M35" t="s">
-        <v>461</v>
+        <v>467</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="M36" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="M37" t="s">
-        <v>466</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A38" t="s">
-        <v>567</v>
-      </c>
-      <c r="M38" s="2" t="s">
-        <v>569</v>
+      <c r="A38" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="M38" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A39" t="s">
-        <v>477</v>
+      <c r="A39" s="1" t="s">
+        <v>458</v>
       </c>
       <c r="M39" t="s">
-        <v>478</v>
+        <v>461</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>459</v>
+      </c>
+      <c r="M40" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>536</v>
+        <v>460</v>
       </c>
       <c r="M41" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.4">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="75" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>538</v>
-      </c>
-      <c r="M42" t="s">
-        <v>537</v>
+        <v>566</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>612</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>539</v>
+        <v>477</v>
       </c>
       <c r="M43" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A44" t="s">
-        <v>540</v>
-      </c>
-      <c r="M44" t="s">
-        <v>467</v>
+        <v>478</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="M45" t="s">
-        <v>468</v>
+        <v>537</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="M46" t="s">
-        <v>111</v>
+        <v>537</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A47" s="1" t="s">
-        <v>545</v>
+      <c r="A47" t="s">
+        <v>539</v>
       </c>
       <c r="M47" t="s">
-        <v>546</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A48" s="1" t="s">
-        <v>547</v>
+      <c r="A48" t="s">
+        <v>540</v>
       </c>
       <c r="M48" t="s">
-        <v>550</v>
+        <v>467</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A49" s="1" t="s">
-        <v>548</v>
+      <c r="A49" t="s">
+        <v>541</v>
       </c>
       <c r="M49" t="s">
-        <v>549</v>
+        <v>468</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
+        <v>542</v>
+      </c>
+      <c r="M50" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A51" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="M51" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="M52" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A53" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="M53" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A54" t="s">
         <v>543</v>
       </c>
-      <c r="M50" t="s">
+      <c r="M54" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A51" t="s">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A55" t="s">
         <v>544</v>
       </c>
-      <c r="M51" t="s">
+      <c r="M55" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A52" t="s">
-        <v>570</v>
-      </c>
-      <c r="M52" s="2" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A53" t="s">
-        <v>581</v>
-      </c>
-      <c r="M53" s="2" t="s">
-        <v>582</v>
+    <row r="56" spans="1:13" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A56" t="s">
+        <v>568</v>
+      </c>
+      <c r="M56" s="2" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A57" t="s">
+        <v>577</v>
+      </c>
+      <c r="M57" s="2" t="s">
+        <v>578</v>
       </c>
     </row>
   </sheetData>
@@ -6004,16 +6165,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131ED9DB-7094-4FCA-8832-3F1005AB8270}">
-  <dimension ref="A1:Q56"/>
+  <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
-    <col min="13" max="13" width="65" customWidth="1"/>
+    <col min="13" max="13" width="55.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.4">
@@ -6066,427 +6227,443 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" ht="54.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>255</v>
-      </c>
-      <c r="M2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
+        <v>620</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="92.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>112</v>
-      </c>
-      <c r="M3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>113</v>
-      </c>
-      <c r="M4" t="s">
-        <v>110</v>
+        <v>622</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>623</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>255</v>
       </c>
       <c r="M5" t="s">
-        <v>467</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="M6" t="s">
-        <v>468</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="M7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="M8" t="s">
-        <v>123</v>
+        <v>467</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="M9" t="s">
-        <v>122</v>
+        <v>468</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M10" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="M11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>227</v>
+        <v>118</v>
       </c>
       <c r="M12" t="s">
-        <v>229</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>228</v>
+        <v>119</v>
       </c>
       <c r="M13" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="37.5" x14ac:dyDescent="0.4">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="64.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>572</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>573</v>
+        <v>120</v>
+      </c>
+      <c r="M14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>227</v>
+      </c>
+      <c r="M15" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
+        <v>228</v>
+      </c>
+      <c r="M16" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>570</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
         <v>382</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M19" t="s">
         <v>383</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A17" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="M17" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A18" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="M18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A19" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="M19" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
-        <v>370</v>
+        <v>381</v>
       </c>
       <c r="M20" t="s">
-        <v>468</v>
+        <v>383</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="M21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="M22" t="s">
-        <v>123</v>
+        <v>467</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="M23" t="s">
-        <v>122</v>
+        <v>468</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="M24" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="M25" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
       <c r="M26" t="s">
-        <v>384</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="M27" t="s">
-        <v>387</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="M28" t="s">
-        <v>386</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
-        <v>400</v>
+        <v>385</v>
       </c>
       <c r="M29" t="s">
-        <v>402</v>
+        <v>384</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
-        <v>401</v>
+        <v>376</v>
       </c>
       <c r="M30" t="s">
-        <v>403</v>
+        <v>387</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="M31" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
-        <v>379</v>
+        <v>400</v>
       </c>
       <c r="M32" t="s">
-        <v>388</v>
+        <v>402</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="M33" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A34" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="M34" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A35" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="M35" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="83.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="M33" t="s">
+      <c r="M36" t="s">
         <v>389</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
-        <v>391</v>
-      </c>
-      <c r="M34" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
-        <v>392</v>
-      </c>
-      <c r="M35" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="64.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A36" t="s">
-        <v>574</v>
-      </c>
-      <c r="M36" s="2" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="M37" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="M38" t="s">
-        <v>397</v>
+        <v>393</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="75" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>571</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>610</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
+        <v>398</v>
+      </c>
+      <c r="M40" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>396</v>
+      </c>
+      <c r="M41" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
         <v>487</v>
       </c>
-      <c r="M40" t="s">
+      <c r="M43" t="s">
         <v>497</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A41" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="M41" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A42" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="M42" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A43" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="M43" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="M44" t="s">
-        <v>468</v>
+        <v>497</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="M45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A46" s="1" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="M46" t="s">
-        <v>123</v>
+        <v>467</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="M47" t="s">
-        <v>122</v>
+        <v>468</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="M48" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="M49" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="M50" t="s">
-        <v>506</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A51" s="1" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="M51" t="s">
-        <v>505</v>
+        <v>124</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="M52" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A53" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="M53" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A54" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="M54" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A55" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="M52" t="s">
+      <c r="M55" t="s">
         <v>509</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A53" t="s">
-        <v>500</v>
-      </c>
-      <c r="M53" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A54" t="s">
-        <v>501</v>
-      </c>
-      <c r="M54" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A55" t="s">
-        <v>575</v>
-      </c>
-      <c r="M55" s="2" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
+        <v>500</v>
+      </c>
+      <c r="M56" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A57" t="s">
+        <v>501</v>
+      </c>
+      <c r="M57" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A58" t="s">
+        <v>572</v>
+      </c>
+      <c r="M58" s="2" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
         <v>502</v>
       </c>
-      <c r="M56" t="s">
+      <c r="M59" t="s">
         <v>503</v>
       </c>
     </row>
@@ -6501,8 +6678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445F46B3-1A86-46EF-9440-E5378C8C2CDD}">
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="L51" sqref="L51"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M53" sqref="M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -6699,10 +6876,10 @@
     </row>
     <row r="19" spans="1:13" ht="120.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
@@ -6939,18 +7116,18 @@
     </row>
     <row r="50" spans="1:13" ht="130.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>612</v>
+        <v>604</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="M51" t="s">
-        <v>599</v>
+        <v>591</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -6963,18 +7140,18 @@
     </row>
     <row r="53" spans="1:13" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>613</v>
+        <v>605</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
-        <v>600</v>
+        <v>592</v>
       </c>
       <c r="M54" t="s">
-        <v>604</v>
+        <v>596</v>
       </c>
     </row>
   </sheetData>
@@ -6988,14 +7165,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA3747E3-550F-4585-A066-931F491B69D2}">
   <dimension ref="A1:Q78"/>
   <sheetViews>
-    <sheetView topLeftCell="D70" workbookViewId="0">
-      <selection activeCell="K77" sqref="K77"/>
+    <sheetView topLeftCell="D22" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="38.375" customWidth="1"/>
-    <col min="13" max="13" width="56" customWidth="1"/>
+    <col min="13" max="13" width="56.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.4">
@@ -7234,10 +7411,10 @@
     </row>
     <row r="25" spans="1:13" ht="75" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>586</v>
+        <v>608</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.4">
@@ -7256,12 +7433,12 @@
         <v>246</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="168.75" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:13" ht="225.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>585</v>
+        <v>609</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.4">
@@ -7440,36 +7617,36 @@
         <v>250</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="98.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:13" ht="132" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" ht="116.25" customHeight="1" x14ac:dyDescent="0.4">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="150.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>591</v>
+        <v>607</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="93.75" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.4">
@@ -7482,10 +7659,10 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.4">
@@ -7626,26 +7803,26 @@
     </row>
     <row r="76" spans="1:13" ht="115.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
       <c r="M76" s="2" t="s">
-        <v>610</v>
+        <v>602</v>
       </c>
     </row>
     <row r="77" spans="1:13" ht="112.5" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="M77" s="2" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
-        <v>602</v>
+        <v>594</v>
       </c>
       <c r="M78" t="s">
-        <v>603</v>
+        <v>595</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat:infooverlay more role info before game start
</commit_message>
<xml_diff>
--- a/transData.xlsx
+++ b/transData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ドキュメント\VisualStudioProject\AmongUs\ExtremeRoles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BDAC21-7F53-4F7A-836E-A91B7EE49999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9EB704-5200-4D32-9291-292880A67F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9495" yWindow="2985" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3315" yWindow="2835" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="676">
   <si>
     <t>English</t>
   </si>
@@ -4817,6 +4817,36 @@
     </rPh>
     <rPh sb="2" eb="4">
       <t>ジンエイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>roleDesc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>役職の詳細</t>
+    <rPh sb="0" eb="2">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ショウサイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>changeRoleMore</t>
+  </si>
+  <si>
+    <t>ページアップ、ページダウンキーで役職切り替え</t>
+    <rPh sb="16" eb="18">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>カ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -5149,10 +5179,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q117"/>
+  <dimension ref="A1:Q120"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView tabSelected="1" topLeftCell="C109" workbookViewId="0">
+      <selection activeCell="M115" sqref="M115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -6055,6 +6085,22 @@
         <v>593</v>
       </c>
     </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A119" t="s">
+        <v>672</v>
+      </c>
+      <c r="M119" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A120" t="s">
+        <v>674</v>
+      </c>
+      <c r="M120" t="s">
+        <v>675</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6066,8 +6112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5C264A-D4F8-4177-9D21-7A3435066086}">
   <dimension ref="A1:Q58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
fix:imposter + crew lover win condition
</commit_message>
<xml_diff>
--- a/transData.xlsx
+++ b/transData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ドキュメント\VisualStudioProject\AmongUs\ExtremeRoles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19274E1C-FC6A-4F76-9395-E02DE7F8E9D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87852D7A-70A7-4C92-B422-D3CFD1587E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4485" yWindow="2430" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -3345,47 +3345,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>相方を殺された恨みで殺人鬼に変化した複数人1組の第三陣営役職
-勝利条件：生存者が同じ組以下になること</t>
-    <rPh sb="3" eb="4">
-      <t>コロ</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>ウラ</t>
-    </rPh>
-    <rPh sb="10" eb="13">
-      <t>サツジンキ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>ヘンカ</t>
-    </rPh>
-    <rPh sb="18" eb="21">
-      <t>フクスウニン</t>
-    </rPh>
-    <rPh sb="22" eb="23">
-      <t>クミ</t>
-    </rPh>
-    <rPh sb="24" eb="28">
-      <t>ダイ</t>
-    </rPh>
-    <rPh sb="31" eb="35">
-      <t>ショウリジョウケン</t>
-    </rPh>
-    <rPh sb="36" eb="39">
-      <t>セイゾンシャ</t>
-    </rPh>
-    <rPh sb="40" eb="41">
-      <t>オナ</t>
-    </rPh>
-    <rPh sb="42" eb="43">
-      <t>クミ</t>
-    </rPh>
-    <rPh sb="43" eb="45">
-      <t>イカ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>SupporterFullDescription</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -3524,67 +3483,6 @@
     </rPh>
     <rPh sb="119" eb="121">
       <t>ヤクショク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>インポスターが誰か分かるクルー役職
-アサシンの特殊能力によって指定された場合、クルー全体の敗北
-インポスターが分かるので会議を主導しつつ身を隠す必要がある
-インポスターに近い設定の役職のため、注意が必要</t>
-    <rPh sb="7" eb="8">
-      <t>ダレ</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>ワ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>ヤクショク</t>
-    </rPh>
-    <rPh sb="23" eb="27">
-      <t>トクシュノウリョク</t>
-    </rPh>
-    <rPh sb="31" eb="33">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="42" eb="44">
-      <t>ゼンタイ</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>ハイボク</t>
-    </rPh>
-    <rPh sb="55" eb="56">
-      <t>ワ</t>
-    </rPh>
-    <rPh sb="60" eb="62">
-      <t>カイギ</t>
-    </rPh>
-    <rPh sb="63" eb="65">
-      <t>シュドウ</t>
-    </rPh>
-    <rPh sb="68" eb="69">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="70" eb="71">
-      <t>カク</t>
-    </rPh>
-    <rPh sb="72" eb="74">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <rPh sb="85" eb="86">
-      <t>チカ</t>
-    </rPh>
-    <rPh sb="87" eb="89">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="90" eb="92">
-      <t>ヤクショク</t>
-    </rPh>
-    <rPh sb="96" eb="98">
-      <t>チュウイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -4415,168 +4313,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>インポスター陣営に新しい勝利条件を追加するインポスター役職
-新しい勝利条件：アサシンの特殊能力でマーリンを当てる
-アサシンの特殊能力：マーリン指定の特殊会議
-マーリン指定の特殊会議：
-　全員が参加するが能力を発動させたアサシン以外投票不可
-　スキップ不可、チャット不可、死亡している人にも投票可
-　投票先がマーリンであればインポスター勝利、それ以外の
-　場合、ゲームが続行(マーリンの能力は継続)
-特殊能力発動条件：追放された場合、自身がキルされた場合の
-処理は設定可
-上記の能力以外は普通のインポスターのため、マーリンを
-探りつつ潜伏し、キルを行う必要がある</t>
-    <rPh sb="6" eb="8">
-      <t>ジンエイ</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>アタラ</t>
-    </rPh>
-    <rPh sb="12" eb="16">
-      <t>ショウリジョウケン</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ツイカ</t>
-    </rPh>
-    <rPh sb="27" eb="29">
-      <t>ヤクショク</t>
-    </rPh>
-    <rPh sb="30" eb="31">
-      <t>アタラ</t>
-    </rPh>
-    <rPh sb="43" eb="47">
-      <t>トクシュノウリョク</t>
-    </rPh>
-    <rPh sb="53" eb="54">
-      <t>ア</t>
-    </rPh>
-    <rPh sb="62" eb="66">
-      <t>トク</t>
-    </rPh>
-    <rPh sb="71" eb="73">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="74" eb="76">
-      <t>トクシュ</t>
-    </rPh>
-    <rPh sb="76" eb="78">
-      <t>カイギ</t>
-    </rPh>
-    <rPh sb="83" eb="85">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="86" eb="88">
-      <t>トクシュ</t>
-    </rPh>
-    <rPh sb="88" eb="90">
-      <t>カイギ</t>
-    </rPh>
-    <rPh sb="93" eb="95">
-      <t>ゼンイン</t>
-    </rPh>
-    <rPh sb="96" eb="98">
-      <t>サンカ</t>
-    </rPh>
-    <rPh sb="101" eb="103">
-      <t>ノウリョク</t>
-    </rPh>
-    <rPh sb="104" eb="106">
-      <t>ハツドウ</t>
-    </rPh>
-    <rPh sb="113" eb="115">
-      <t>イガイ</t>
-    </rPh>
-    <rPh sb="115" eb="117">
-      <t>トウヒョウ</t>
-    </rPh>
-    <rPh sb="117" eb="119">
-      <t>フカ</t>
-    </rPh>
-    <rPh sb="125" eb="127">
-      <t>フカ</t>
-    </rPh>
-    <rPh sb="132" eb="134">
-      <t>フカ</t>
-    </rPh>
-    <rPh sb="135" eb="137">
-      <t>シボウ</t>
-    </rPh>
-    <rPh sb="141" eb="142">
-      <t>ヒト</t>
-    </rPh>
-    <rPh sb="144" eb="146">
-      <t>トウヒョウ</t>
-    </rPh>
-    <rPh sb="146" eb="147">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="149" eb="151">
-      <t>トウヒョウ</t>
-    </rPh>
-    <rPh sb="151" eb="152">
-      <t>サキ</t>
-    </rPh>
-    <rPh sb="167" eb="169">
-      <t>ショウリ</t>
-    </rPh>
-    <rPh sb="172" eb="174">
-      <t>イガイ</t>
-    </rPh>
-    <rPh sb="177" eb="179">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="184" eb="186">
-      <t>ゾッコウ</t>
-    </rPh>
-    <rPh sb="192" eb="194">
-      <t>ノウリョク</t>
-    </rPh>
-    <rPh sb="195" eb="197">
-      <t>ケイゾク</t>
-    </rPh>
-    <rPh sb="199" eb="203">
-      <t>トクシュ</t>
-    </rPh>
-    <rPh sb="203" eb="207">
-      <t>ハツドウジョウケン</t>
-    </rPh>
-    <rPh sb="208" eb="210">
-      <t>ツイホウ</t>
-    </rPh>
-    <rPh sb="213" eb="215">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="224" eb="226">
-      <t>バアイショリ</t>
-    </rPh>
-    <rPh sb="235" eb="237">
-      <t>ジョウキ</t>
-    </rPh>
-    <rPh sb="238" eb="240">
-      <t>ノウリョク</t>
-    </rPh>
-    <rPh sb="240" eb="242">
-      <t>イガイ</t>
-    </rPh>
-    <rPh sb="243" eb="245">
-      <t>フツウ</t>
-    </rPh>
-    <rPh sb="262" eb="263">
-      <t>サグ</t>
-    </rPh>
-    <rPh sb="266" eb="268">
-      <t>センプク</t>
-    </rPh>
-    <rPh sb="273" eb="274">
-      <t>オコナ</t>
-    </rPh>
-    <rPh sb="275" eb="277">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>複数人1組の第三陣営役職
 勝利条件1：生存者が同じ組以下になること、ただし、
 インポスターや第三陣営でキル能力を持っている人が
@@ -4639,11 +4375,243 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>NeetHasTask</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>タスクを持つか</t>
+    <rPh sb="4" eb="5">
+      <t>モ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>第三陣営か</t>
+    <rPh sb="0" eb="2">
+      <t>ダイサン</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ジンエイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>roleDesc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>役職の詳細</t>
+    <rPh sb="0" eb="2">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ショウサイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>changeRoleMore</t>
+  </si>
+  <si>
+    <t>gameReplace</t>
+  </si>
+  <si>
+    <t>※ゲーム開始時、もしくはゲーム中に判明</t>
+    <rPh sb="4" eb="6">
+      <t>カイシ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ジ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>チュウ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ハンメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PgUpキー、PgDnキーで役職切り替え</t>
+    <rPh sb="14" eb="16">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>カ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Assassinate</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DeadAssassinate</t>
+  </si>
+  <si>
+    <t>暗殺</t>
+    <rPh sb="0" eb="2">
+      <t>アンサツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>除外</t>
+    <rPh sb="0" eb="2">
+      <t>ジョガイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>version</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>developer</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Developed by </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>debugThunk</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>デバッグ協力：</t>
+    <rPh sb="4" eb="6">
+      <t>キョウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MOD開発：</t>
+    <rPh sb="3" eb="5">
+      <t>カイハツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ver.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Version:</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>複数人1組のクルー役職
+勝利条件1：クルー勝利、ただし、同じ組で別陣営の人が居た場合
+その人は敗北
+勝利条件2：他の生存者が同じ組以下になり、同じ組のタスクが
+全て終了すること(この勝利条件は同じ組で別陣営の人がいる場合
+のみ有効になる)
+勝利条件3：以下条件の全てを満たした場合
+　①：他の生存者が同じ組以下
+　②：インポスターの生存者が0
+　③：同じ組の中に別陣営の人が居る
+　④：他の生存者全てがクルーもしくは
+　　　③の別陣営の人と同じ組である
+同じ組の人が一定数以下になると自決もしくは第三陣営に
+変化する
+自決を行う人数は設定により変化する</t>
+    <rPh sb="0" eb="3">
+      <t>フクスウニン</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>クミ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>ベツ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ジンエイ</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="56" eb="57">
+      <t>ホカ</t>
+    </rPh>
+    <rPh sb="120" eb="124">
+      <t>ショウリジョウケン</t>
+    </rPh>
+    <rPh sb="126" eb="128">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="128" eb="130">
+      <t>ジョウケン</t>
+    </rPh>
+    <rPh sb="131" eb="132">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="134" eb="135">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="138" eb="140">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="144" eb="145">
+      <t>ホカ</t>
+    </rPh>
+    <rPh sb="146" eb="149">
+      <t>セイゾンシャ</t>
+    </rPh>
+    <rPh sb="150" eb="151">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="152" eb="153">
+      <t>クミ</t>
+    </rPh>
+    <rPh sb="153" eb="155">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="166" eb="169">
+      <t>セイゾンシャ</t>
+    </rPh>
+    <rPh sb="193" eb="194">
+      <t>ホカ</t>
+    </rPh>
+    <rPh sb="198" eb="199">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="214" eb="217">
+      <t>ベツ</t>
+    </rPh>
+    <rPh sb="218" eb="219">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="220" eb="221">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="222" eb="223">
+      <t>クミ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>複数人1組のインポスター役職
 勝利条件1：インポスター勝利、ただし、同じ組で別陣営の人が
 居た場合、その人は敗北
 勝利条件2：生存者が同じ組以下になり、同じ組のタスクが全て
 終了すること(この勝利条件は同じ組で別陣営の人がいる場合のみ有効になる)
+勝利条件3：以下の全てを満たした場合
+　①：他の生存者が同じ組以下
+　②：同じ組の中に別陣営の人が居る
+　③：他の全ての生存者がクルーもしくはインポスターである
 同じ組の人が一定数以下になると自決もしくは第三陣営に
 変化する
 自決を行う人数は設定により変化する</t>
@@ -4683,249 +4651,316 @@
     <rPh sb="117" eb="119">
       <t>ユウコウ</t>
     </rPh>
-    <rPh sb="124" eb="125">
+    <rPh sb="181" eb="182">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="205" eb="206">
       <t>オナ</t>
     </rPh>
-    <rPh sb="126" eb="127">
+    <rPh sb="207" eb="208">
       <t>クミ</t>
     </rPh>
-    <rPh sb="128" eb="129">
+    <rPh sb="209" eb="210">
       <t>ヒト</t>
     </rPh>
-    <rPh sb="130" eb="133">
+    <rPh sb="211" eb="214">
       <t>イッテイスウ</t>
     </rPh>
-    <rPh sb="133" eb="135">
+    <rPh sb="214" eb="216">
       <t>イカ</t>
     </rPh>
-    <rPh sb="139" eb="141">
+    <rPh sb="220" eb="222">
       <t>ジケツ</t>
     </rPh>
-    <rPh sb="145" eb="149">
+    <rPh sb="226" eb="230">
       <t>ダイ</t>
     </rPh>
-    <rPh sb="151" eb="153">
+    <rPh sb="232" eb="234">
       <t>ヘンカ</t>
     </rPh>
-    <rPh sb="156" eb="158">
+    <rPh sb="237" eb="239">
       <t>ジケツ</t>
     </rPh>
-    <rPh sb="159" eb="160">
+    <rPh sb="240" eb="241">
       <t>オコナ</t>
     </rPh>
-    <rPh sb="161" eb="163">
+    <rPh sb="242" eb="244">
       <t>ニンズウ</t>
     </rPh>
+    <rPh sb="245" eb="247">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="250" eb="252">
+      <t>ヘンカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>相方を殺された恨みで殺人鬼に変化した複数人1組の第三陣営役職
+勝利条件：自分以外を皆殺しにする</t>
+    <rPh sb="3" eb="4">
+      <t>コロ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ウラ</t>
+    </rPh>
+    <rPh sb="10" eb="13">
+      <t>サツジンキ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ヘンカ</t>
+    </rPh>
+    <rPh sb="18" eb="21">
+      <t>フクスウニン</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>クミ</t>
+    </rPh>
+    <rPh sb="24" eb="28">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="31" eb="35">
+      <t>ショウリジョウケン</t>
+    </rPh>
+    <rPh sb="36" eb="40">
+      <t>ジブンイガイ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>ミナゴロ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>インポスターが誰か分かるクルー役職
+アサシンと一対の関係である。
+アサシンがアサインされない場合、この役職もアサインされない
+アサシンの特殊能力によって指定された場合、クルー全体の敗北
+インポスターが分かるので会議を主導しつつ身を隠す必要がある
+インポスターに近い設定の役職のため、注意が必要</t>
+    <rPh sb="7" eb="8">
+      <t>ダレ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>ワ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>イッツイ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>カンケイ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="68" eb="72">
+      <t>トクシュノウリョク</t>
+    </rPh>
+    <rPh sb="76" eb="78">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="81" eb="83">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="87" eb="89">
+      <t>ゼンタイ</t>
+    </rPh>
+    <rPh sb="90" eb="92">
+      <t>ハイボク</t>
+    </rPh>
+    <rPh sb="100" eb="101">
+      <t>ワ</t>
+    </rPh>
+    <rPh sb="105" eb="107">
+      <t>カイギ</t>
+    </rPh>
+    <rPh sb="108" eb="110">
+      <t>シュドウ</t>
+    </rPh>
+    <rPh sb="113" eb="114">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="115" eb="116">
+      <t>カク</t>
+    </rPh>
+    <rPh sb="117" eb="119">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="130" eb="131">
+      <t>チカ</t>
+    </rPh>
+    <rPh sb="132" eb="134">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="135" eb="137">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="141" eb="143">
+      <t>チュウイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>インポスター陣営に新しい勝利条件を追加するインポスター役職
+マーリンと一対の関係である。
+マーリンがアサインされない場合、この役職もアサインされない
+新しい勝利条件：アサシンの特殊能力でマーリンを当てる
+アサシンの特殊能力：特殊会議「マーリンは誰だ？」
+特殊会議「マーリンは誰だ？」：
+　全員が参加するが能力を発動させたアサシン以外投票不可
+　スキップ不可、チャット不可、死亡している人にも投票可
+　投票先がマーリンであればインポスター勝利、それ以外の
+　場合、ゲームが続行(マーリンの能力は継続)
+特殊能力発動条件：追放された場合、自身がキルされた場合の
+処理は設定により変化する
+上記の能力以外は普通のインポスターのため、マーリンを
+探りつつ潜伏し、キルを行う必要がある</t>
+    <rPh sb="6" eb="8">
+      <t>ジンエイ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>アタラ</t>
+    </rPh>
+    <rPh sb="12" eb="16">
+      <t>ショウリジョウケン</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ツイカ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="75" eb="76">
+      <t>アタラ</t>
+    </rPh>
+    <rPh sb="88" eb="92">
+      <t>トクシュノウリョク</t>
+    </rPh>
+    <rPh sb="98" eb="99">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="107" eb="111">
+      <t>トク</t>
+    </rPh>
+    <rPh sb="112" eb="114">
+      <t>トクシュ</t>
+    </rPh>
+    <rPh sb="114" eb="116">
+      <t>カイギ</t>
+    </rPh>
+    <rPh sb="122" eb="123">
+      <t>ダレ</t>
+    </rPh>
+    <rPh sb="144" eb="146">
+      <t>ゼンイン</t>
+    </rPh>
+    <rPh sb="147" eb="149">
+      <t>サンカ</t>
+    </rPh>
+    <rPh sb="152" eb="154">
+      <t>ノウリョク</t>
+    </rPh>
+    <rPh sb="155" eb="157">
+      <t>ハツドウ</t>
+    </rPh>
     <rPh sb="164" eb="166">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="169" eb="171">
+      <t>イガイ</t>
+    </rPh>
+    <rPh sb="166" eb="168">
+      <t>トウヒョウ</t>
+    </rPh>
+    <rPh sb="168" eb="170">
+      <t>フカ</t>
+    </rPh>
+    <rPh sb="176" eb="178">
+      <t>フカ</t>
+    </rPh>
+    <rPh sb="183" eb="185">
+      <t>フカ</t>
+    </rPh>
+    <rPh sb="186" eb="188">
+      <t>シボウ</t>
+    </rPh>
+    <rPh sb="192" eb="193">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="195" eb="197">
+      <t>トウヒョウ</t>
+    </rPh>
+    <rPh sb="197" eb="198">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="200" eb="202">
+      <t>トウヒョウ</t>
+    </rPh>
+    <rPh sb="202" eb="203">
+      <t>サキ</t>
+    </rPh>
+    <rPh sb="218" eb="220">
+      <t>ショウリ</t>
+    </rPh>
+    <rPh sb="223" eb="225">
+      <t>イガイ</t>
+    </rPh>
+    <rPh sb="228" eb="230">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="235" eb="237">
+      <t>ゾッコウ</t>
+    </rPh>
+    <rPh sb="243" eb="245">
+      <t>ノウリョク</t>
+    </rPh>
+    <rPh sb="246" eb="248">
+      <t>ケイゾク</t>
+    </rPh>
+    <rPh sb="250" eb="254">
+      <t>トクシュ</t>
+    </rPh>
+    <rPh sb="254" eb="258">
+      <t>ハツドウジョウケン</t>
+    </rPh>
+    <rPh sb="259" eb="261">
+      <t>ツイホウ</t>
+    </rPh>
+    <rPh sb="264" eb="266">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="275" eb="277">
+      <t>バアイショリ</t>
+    </rPh>
+    <rPh sb="287" eb="289">
       <t>ヘンカ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>複数人1組のクルー役職
-勝利条件1：クルー勝利、ただし、同じ組で別陣営の人が居た場合
-その人は敗北
-勝利条件2：生存者が同じ組以下になり、同じ組のタスクが
-全て終了すること(この勝利条件は同じ組で別陣営の人がいる場合
-のみ有効になる)
-同じ組の人が一定数以下になると自決もしくは第三陣営に
-変化する
-自決を行う人数は設定により変化する</t>
-    <rPh sb="0" eb="3">
-      <t>フクスウニン</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>クミ</t>
-    </rPh>
-    <rPh sb="32" eb="33">
-      <t>ベツ</t>
-    </rPh>
-    <rPh sb="33" eb="35">
-      <t>ジンエイ</t>
-    </rPh>
-    <rPh sb="36" eb="37">
-      <t>ヒト</t>
-    </rPh>
-    <rPh sb="38" eb="39">
-      <t>イ</t>
-    </rPh>
-    <rPh sb="40" eb="42">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="45" eb="46">
-      <t>ヒト</t>
-    </rPh>
-    <rPh sb="118" eb="119">
-      <t>オナ</t>
-    </rPh>
-    <rPh sb="120" eb="121">
-      <t>クミ</t>
-    </rPh>
-    <rPh sb="122" eb="123">
-      <t>ヒト</t>
-    </rPh>
-    <rPh sb="124" eb="127">
-      <t>イッテイスウ</t>
-    </rPh>
-    <rPh sb="127" eb="129">
-      <t>イカ</t>
-    </rPh>
-    <rPh sb="133" eb="135">
-      <t>ジケツ</t>
-    </rPh>
-    <rPh sb="139" eb="143">
-      <t>ダイ</t>
-    </rPh>
-    <rPh sb="145" eb="147">
-      <t>ヘンカ</t>
-    </rPh>
-    <rPh sb="150" eb="152">
-      <t>ジケツ</t>
-    </rPh>
-    <rPh sb="153" eb="154">
+    <rPh sb="292" eb="294">
+      <t>ジョウキ</t>
+    </rPh>
+    <rPh sb="295" eb="297">
+      <t>ノウリョク</t>
+    </rPh>
+    <rPh sb="297" eb="299">
+      <t>イガイ</t>
+    </rPh>
+    <rPh sb="300" eb="302">
+      <t>フツウ</t>
+    </rPh>
+    <rPh sb="319" eb="320">
+      <t>サグ</t>
+    </rPh>
+    <rPh sb="323" eb="325">
+      <t>センプク</t>
+    </rPh>
+    <rPh sb="330" eb="331">
       <t>オコナ</t>
     </rPh>
-    <rPh sb="155" eb="157">
-      <t>ニンズウ</t>
-    </rPh>
-    <rPh sb="158" eb="160">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="163" eb="165">
-      <t>ヘンカ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>NeetHasTask</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>タスクを持つか</t>
-    <rPh sb="4" eb="5">
-      <t>モ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>第三陣営か</t>
-    <rPh sb="0" eb="2">
-      <t>ダイサン</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ジンエイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>roleDesc</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>役職の詳細</t>
-    <rPh sb="0" eb="2">
-      <t>ヤクショク</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ショウサイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>changeRoleMore</t>
-  </si>
-  <si>
-    <t>gameReplace</t>
-  </si>
-  <si>
-    <t>※ゲーム開始時、もしくはゲーム中に判明</t>
-    <rPh sb="4" eb="6">
-      <t>カイシ</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>ジ</t>
-    </rPh>
-    <rPh sb="15" eb="16">
-      <t>チュウ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ハンメイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>PgUpキー、PgDnキーで役職切り替え</t>
-    <rPh sb="14" eb="16">
-      <t>ヤクショク</t>
-    </rPh>
-    <rPh sb="16" eb="17">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="18" eb="19">
-      <t>カ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Assassinate</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>DeadAssassinate</t>
-  </si>
-  <si>
-    <t>暗殺</t>
-    <rPh sb="0" eb="2">
-      <t>アンサツ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>除外</t>
-    <rPh sb="0" eb="2">
-      <t>ジョガイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>version</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>developer</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Developed by </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>debugThunk</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>デバッグ協力：</t>
-    <rPh sb="4" eb="6">
-      <t>キョウリョク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>MOD開発：</t>
-    <rPh sb="3" eb="5">
-      <t>カイハツ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ver.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Version:</t>
+    <rPh sb="332" eb="334">
+      <t>ヒツヨウ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5259,7 +5294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E34" workbookViewId="0">
+    <sheetView topLeftCell="E109" workbookViewId="0">
       <selection activeCell="M50" sqref="M50"/>
     </sheetView>
   </sheetViews>
@@ -5711,32 +5746,32 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="B49" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="M49" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
       <c r="B50" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
       <c r="M50" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="M51" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.4">
@@ -6043,18 +6078,18 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A100" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="M100" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A101" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="M101" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.4">
@@ -6195,42 +6230,42 @@
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A126" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="M126" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A127" t="s">
+        <v>591</v>
+      </c>
+      <c r="M127" t="s">
         <v>592</v>
-      </c>
-      <c r="M127" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A129" t="s">
-        <v>672</v>
+        <v>667</v>
       </c>
       <c r="M129" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A130" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
       <c r="M130" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A132" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="M132" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
     </row>
   </sheetData>
@@ -6244,8 +6279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5C264A-D4F8-4177-9D21-7A3435066086}">
   <dimension ref="A1:Q58"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -6306,26 +6341,26 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="M2" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="M3" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="57" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="41.25" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -6361,7 +6396,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>106</v>
       </c>
@@ -6393,7 +6428,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:17" ht="39" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>561</v>
       </c>
@@ -6518,7 +6553,7 @@
         <v>562</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.4">
@@ -6569,7 +6604,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
         <v>456</v>
       </c>
@@ -6606,7 +6641,7 @@
         <v>564</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.4">
@@ -6683,10 +6718,10 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
       <c r="M53" t="s">
-        <v>670</v>
+        <v>665</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.4">
@@ -6694,7 +6729,7 @@
         <v>547</v>
       </c>
       <c r="M54" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.4">
@@ -6802,18 +6837,18 @@
     </row>
     <row r="2" spans="1:17" ht="54.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="92.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.4">
@@ -6917,7 +6952,7 @@
         <v>568</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.4">
@@ -7085,7 +7120,7 @@
         <v>569</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.4">
@@ -7242,23 +7277,23 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="M61" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A62" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="M62" t="s">
         <v>621</v>
-      </c>
-      <c r="M62" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A63" s="1" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="M63" t="s">
         <v>110</v>
@@ -7266,7 +7301,7 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A64" s="1" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="M64" t="s">
         <v>466</v>
@@ -7274,7 +7309,7 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A65" s="1" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="M65" t="s">
         <v>467</v>
@@ -7282,7 +7317,7 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A66" s="1" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="M66" t="s">
         <v>111</v>
@@ -7290,7 +7325,7 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A67" s="1" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="M67" t="s">
         <v>123</v>
@@ -7298,7 +7333,7 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A68" s="1" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="M68" t="s">
         <v>122</v>
@@ -7306,7 +7341,7 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A69" s="1" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="M69" t="s">
         <v>124</v>
@@ -7314,7 +7349,7 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A70" s="1" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="M70" t="s">
         <v>125</v>
@@ -7322,71 +7357,71 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A71" s="1" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="M71" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A72" s="1" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="M72" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A73" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="M73" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="M74" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
+        <v>627</v>
+      </c>
+      <c r="M75" t="s">
         <v>629</v>
-      </c>
-      <c r="M75" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="76" spans="1:13" ht="135.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="M76" s="2" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="M78" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A79" s="1" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="M79" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="M80" t="s">
         <v>110</v>
@@ -7394,7 +7429,7 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A81" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="M81" t="s">
         <v>466</v>
@@ -7402,7 +7437,7 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A82" s="1" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="M82" t="s">
         <v>467</v>
@@ -7410,7 +7445,7 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A83" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="M83" t="s">
         <v>111</v>
@@ -7418,7 +7453,7 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A84" s="1" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="M84" t="s">
         <v>123</v>
@@ -7426,7 +7461,7 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A85" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="M85" t="s">
         <v>122</v>
@@ -7434,7 +7469,7 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A86" s="1" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="M86" t="s">
         <v>124</v>
@@ -7442,7 +7477,7 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A87" s="1" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="M87" t="s">
         <v>125</v>
@@ -7450,66 +7485,66 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A88" s="1" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="M88" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A89" s="1" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="M89" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A90" s="1" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="M90" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A91" s="1" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="M91" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A92" s="1" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="M92" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="M93" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="M94" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="95" spans="1:13" ht="96" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A95" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="M95" s="2" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
   </sheetData>
@@ -7964,15 +7999,15 @@
         <v>573</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
+        <v>586</v>
+      </c>
+      <c r="M51" t="s">
         <v>587</v>
-      </c>
-      <c r="M51" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -7985,10 +8020,10 @@
     </row>
     <row r="53" spans="1:13" ht="75" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
   </sheetData>
@@ -8002,8 +8037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA3747E3-550F-4585-A066-931F491B69D2}">
   <dimension ref="A1:Q77"/>
   <sheetViews>
-    <sheetView topLeftCell="C74" workbookViewId="0">
-      <selection activeCell="M76" sqref="M76"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -8246,12 +8281,12 @@
         <v>243</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="75" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:13" ht="111.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>577</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>596</v>
+        <v>688</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.4">
@@ -8270,12 +8305,12 @@
         <v>246</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="225.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:13" ht="273.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>578</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>665</v>
+        <v>689</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.4">
@@ -8283,7 +8318,7 @@
         <v>347</v>
       </c>
       <c r="M29" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.4">
@@ -8454,20 +8489,20 @@
         <v>250</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="132.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:13" ht="280.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>579</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" ht="177.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="243.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>581</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>667</v>
+        <v>686</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="154.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -8475,7 +8510,7 @@
         <v>580</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -8483,7 +8518,7 @@
         <v>582</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>583</v>
+        <v>687</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.4">
@@ -8496,10 +8531,10 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
+        <v>588</v>
+      </c>
+      <c r="M57" s="2" t="s">
         <v>589</v>
-      </c>
-      <c r="M57" s="2" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.4">
@@ -8638,20 +8673,20 @@
         <v>529</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="177.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:13" ht="170.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="M76" s="2" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="77" spans="1:13" ht="168.75" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="M77" s="2" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat:assassin new final status
</commit_message>
<xml_diff>
--- a/transData.xlsx
+++ b/transData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ドキュメント\VisualStudioProject\AmongUs\ExtremeRoles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87852D7A-70A7-4C92-B422-D3CFD1587E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19ABF5E4-38B9-4261-8C6B-D5A800041B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="692">
   <si>
     <t>English</t>
   </si>
@@ -4960,6 +4960,17 @@
     </rPh>
     <rPh sb="332" eb="334">
       <t>ヒツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Surrender</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>降伏</t>
+    <rPh sb="0" eb="2">
+      <t>コウフク</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -5292,10 +5303,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q132"/>
+  <dimension ref="A1:Q133"/>
   <sheetViews>
-    <sheetView topLeftCell="E109" workbookViewId="0">
-      <selection activeCell="M50" sqref="M50"/>
+    <sheetView tabSelected="1" topLeftCell="C86" workbookViewId="0">
+      <selection activeCell="M99" sqref="M99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -6092,179 +6103,187 @@
         <v>676</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A103" t="s">
-        <v>552</v>
-      </c>
-      <c r="M103" t="s">
-        <v>553</v>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A102" t="s">
+        <v>690</v>
+      </c>
+      <c r="M102" t="s">
+        <v>691</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A104" t="s">
+        <v>552</v>
+      </c>
+      <c r="M104" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A105" t="s">
         <v>551</v>
       </c>
-      <c r="M104" t="s">
+      <c r="M105" t="s">
         <v>554</v>
-      </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A106" t="s">
-        <v>337</v>
-      </c>
-      <c r="M106" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A107" t="s">
+        <v>337</v>
+      </c>
+      <c r="M107" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A108" t="s">
         <v>338</v>
       </c>
-      <c r="M107" t="s">
+      <c r="M108" t="s">
         <v>419</v>
-      </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A109" t="s">
-        <v>443</v>
-      </c>
-      <c r="M109" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A110" t="s">
+        <v>443</v>
+      </c>
+      <c r="M110" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A111" t="s">
         <v>442</v>
       </c>
-      <c r="M110" t="s">
+      <c r="M111" t="s">
         <v>444</v>
-      </c>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A112" t="s">
-        <v>268</v>
-      </c>
-      <c r="M112" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A113" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="M113" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A114" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="M114" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A115" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="M115" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A116" t="s">
+        <v>271</v>
+      </c>
+      <c r="M116" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A117" t="s">
         <v>272</v>
       </c>
-      <c r="M116" t="s">
+      <c r="M117" t="s">
         <v>274</v>
-      </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A118" t="s">
-        <v>359</v>
-      </c>
-      <c r="M118" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A119" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="M119" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A120" t="s">
+        <v>358</v>
+      </c>
+      <c r="M120" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A121" t="s">
         <v>345</v>
       </c>
-      <c r="M120" t="s">
+      <c r="M121" t="s">
         <v>346</v>
-      </c>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A122" t="s">
-        <v>555</v>
-      </c>
-      <c r="M122" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A123" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="M123" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A124" t="s">
+        <v>557</v>
+      </c>
+      <c r="M124" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A125" t="s">
         <v>559</v>
       </c>
-      <c r="M124" t="s">
+      <c r="M125" t="s">
         <v>560</v>
-      </c>
-    </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A126" t="s">
-        <v>590</v>
-      </c>
-      <c r="M126" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A127" t="s">
+        <v>590</v>
+      </c>
+      <c r="M127" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A128" t="s">
         <v>591</v>
       </c>
-      <c r="M127" t="s">
+      <c r="M128" t="s">
         <v>592</v>
-      </c>
-    </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A129" t="s">
-        <v>667</v>
-      </c>
-      <c r="M129" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A130" t="s">
+        <v>667</v>
+      </c>
+      <c r="M130" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A131" t="s">
         <v>669</v>
       </c>
-      <c r="M130" t="s">
+      <c r="M131" t="s">
         <v>672</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A132" t="s">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A133" t="s">
         <v>670</v>
       </c>
-      <c r="M132" t="s">
+      <c r="M133" t="s">
         <v>671</v>
       </c>
     </row>
@@ -8037,7 +8056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA3747E3-550F-4585-A066-931F491B69D2}">
   <dimension ref="A1:Q77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+    <sheetView topLeftCell="A89" workbookViewId="0">
       <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat:hide name plate option
</commit_message>
<xml_diff>
--- a/transData.xlsx
+++ b/transData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ドキュメント\VisualStudioProject\AmongUs\ExtremeRoles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4F39DE-E5F5-46A0-B973-7FD78C6DD7AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6B1ED7-CD90-4970-9C08-19B176DDE4D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="708">
   <si>
     <t>English</t>
   </si>
@@ -4915,6 +4915,20 @@
     </rPh>
     <rPh sb="12" eb="13">
       <t>ウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>hideNamePlateButton</t>
+  </si>
+  <si>
+    <t>Hide Nameplate</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ネームプレートを非表示にする</t>
+    <rPh sb="8" eb="11">
+      <t>ヒヒョウジ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -5247,10 +5261,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q133"/>
+  <dimension ref="A1:Q134"/>
   <sheetViews>
-    <sheetView topLeftCell="C86" workbookViewId="0">
-      <selection activeCell="M99" sqref="M99"/>
+    <sheetView tabSelected="1" topLeftCell="C118" workbookViewId="0">
+      <selection activeCell="M127" sqref="M127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -5627,343 +5641,354 @@
         <v>296</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A37" t="s">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
+        <v>705</v>
+      </c>
+      <c r="B36" t="s">
+        <v>706</v>
+      </c>
+      <c r="M36" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
         <v>440</v>
       </c>
-      <c r="M37" t="s">
+      <c r="M38" t="s">
         <v>441</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A39" t="s">
-        <v>286</v>
-      </c>
-      <c r="M39" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="M40" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="M41" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
+        <v>289</v>
+      </c>
+      <c r="M42" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
         <v>291</v>
       </c>
-      <c r="M42" t="s">
+      <c r="M43" t="s">
         <v>295</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A44" t="s">
-        <v>287</v>
-      </c>
-      <c r="M44" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="M45" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="M46" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
+        <v>292</v>
+      </c>
+      <c r="M47" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
         <v>293</v>
       </c>
-      <c r="M47" t="s">
+      <c r="M48" t="s">
         <v>294</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A49" t="s">
-        <v>637</v>
-      </c>
-      <c r="B49" t="s">
-        <v>644</v>
-      </c>
-      <c r="M49" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B50" t="s">
-        <v>639</v>
+        <v>644</v>
       </c>
       <c r="M50" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
+        <v>638</v>
+      </c>
+      <c r="B51" t="s">
+        <v>639</v>
+      </c>
+      <c r="M51" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A52" t="s">
         <v>640</v>
       </c>
-      <c r="M51" t="s">
+      <c r="M52" t="s">
         <v>641</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A57" t="s">
-        <v>413</v>
-      </c>
-      <c r="M57" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="M58" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
+        <v>411</v>
+      </c>
+      <c r="M59" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A60" t="s">
         <v>412</v>
       </c>
-      <c r="M59" t="s">
+      <c r="M60" t="s">
         <v>302</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A61" t="s">
-        <v>69</v>
-      </c>
-      <c r="B61" t="s">
-        <v>70</v>
-      </c>
-      <c r="M61" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
+        <v>69</v>
+      </c>
+      <c r="B62" t="s">
+        <v>70</v>
+      </c>
+      <c r="M62" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A63" t="s">
         <v>72</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>73</v>
       </c>
-      <c r="M62" t="s">
+      <c r="M63" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A64" t="s">
-        <v>97</v>
-      </c>
-      <c r="B64" t="s">
-        <v>98</v>
-      </c>
-      <c r="M64" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B65" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M65" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
+        <v>95</v>
+      </c>
+      <c r="B66" t="s">
+        <v>99</v>
+      </c>
+      <c r="M66" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A67" t="s">
         <v>96</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>100</v>
       </c>
-      <c r="M66" t="s">
+      <c r="M67" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A68" t="s">
-        <v>76</v>
-      </c>
-      <c r="B68" t="s">
-        <v>77</v>
-      </c>
-      <c r="M68" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B69" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M69" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
+        <v>78</v>
+      </c>
+      <c r="B70" t="s">
+        <v>79</v>
+      </c>
+      <c r="M70" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A71" t="s">
         <v>80</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B71" t="s">
         <v>81</v>
       </c>
-      <c r="M70" t="s">
+      <c r="M71" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A72" t="s">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A73" t="s">
         <v>82</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B73" t="s">
         <v>83</v>
       </c>
-      <c r="M72" t="s">
+      <c r="M73" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A74" t="s">
-        <v>246</v>
-      </c>
-      <c r="B74" t="s">
-        <v>247</v>
-      </c>
-      <c r="M74" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
+        <v>246</v>
+      </c>
+      <c r="B75" t="s">
+        <v>247</v>
+      </c>
+      <c r="M75" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A76" t="s">
         <v>248</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B76" t="s">
         <v>249</v>
       </c>
-      <c r="M75" t="s">
+      <c r="M76" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A77" t="s">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A78" t="s">
         <v>250</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B78" t="s">
         <v>251</v>
       </c>
-      <c r="M77" t="s">
+      <c r="M78" t="s">
         <v>252</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A79" t="s">
-        <v>253</v>
-      </c>
-      <c r="B79" t="s">
-        <v>254</v>
-      </c>
-      <c r="M79" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B80" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="M80" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
-        <v>303</v>
+        <v>256</v>
       </c>
       <c r="B81" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="M81" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
-        <v>260</v>
+        <v>303</v>
       </c>
       <c r="B82" t="s">
         <v>259</v>
       </c>
       <c r="M82" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
-        <v>329</v>
+        <v>260</v>
       </c>
       <c r="B83" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="M83" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
+        <v>329</v>
+      </c>
+      <c r="B84" t="s">
+        <v>261</v>
+      </c>
+      <c r="M84" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A85" t="s">
         <v>330</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B85" t="s">
         <v>331</v>
       </c>
-      <c r="M84" t="s">
+      <c r="M85" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A87" t="s">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A88" t="s">
         <v>307</v>
       </c>
-      <c r="M87" t="s">
+      <c r="M88" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A89" t="s">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A90" t="s">
         <v>386</v>
       </c>
-      <c r="M89" t="s">
+      <c r="M90" t="s">
         <v>387</v>
       </c>
     </row>
@@ -5975,259 +6000,259 @@
         <v>416</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A93" t="s">
-        <v>373</v>
-      </c>
-      <c r="M93" t="s">
-        <v>383</v>
-      </c>
-    </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="M94" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A95" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="M95" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A96" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="M96" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A97" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="M97" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="M98" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
-        <v>414</v>
+        <v>378</v>
       </c>
       <c r="M99" t="s">
-        <v>415</v>
+        <v>379</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A100" t="s">
-        <v>633</v>
+        <v>414</v>
       </c>
       <c r="M100" t="s">
-        <v>635</v>
+        <v>415</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A101" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="M101" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A102" t="s">
+        <v>634</v>
+      </c>
+      <c r="M102" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A103" t="s">
         <v>650</v>
       </c>
-      <c r="M102" t="s">
+      <c r="M103" t="s">
         <v>651</v>
-      </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A104" t="s">
-        <v>512</v>
-      </c>
-      <c r="M104" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A105" t="s">
+        <v>512</v>
+      </c>
+      <c r="M105" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A106" t="s">
         <v>511</v>
       </c>
-      <c r="M105" t="s">
+      <c r="M106" t="s">
         <v>514</v>
-      </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A107" t="s">
-        <v>304</v>
-      </c>
-      <c r="M107" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A108" t="s">
+        <v>304</v>
+      </c>
+      <c r="M108" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A109" t="s">
         <v>305</v>
       </c>
-      <c r="M108" t="s">
+      <c r="M109" t="s">
         <v>385</v>
-      </c>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A110" t="s">
-        <v>409</v>
-      </c>
-      <c r="M110" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A111" t="s">
+        <v>409</v>
+      </c>
+      <c r="M111" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A112" t="s">
         <v>408</v>
       </c>
-      <c r="M111" t="s">
+      <c r="M112" t="s">
         <v>410</v>
-      </c>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A113" t="s">
-        <v>239</v>
-      </c>
-      <c r="M113" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A114" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="M114" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A115" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="M115" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A116" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M116" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A117" t="s">
+        <v>242</v>
+      </c>
+      <c r="M117" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A118" t="s">
         <v>243</v>
       </c>
-      <c r="M117" t="s">
+      <c r="M118" t="s">
         <v>245</v>
-      </c>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A119" t="s">
-        <v>325</v>
-      </c>
-      <c r="M119" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A120" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="M120" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A121" t="s">
+        <v>324</v>
+      </c>
+      <c r="M121" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A122" t="s">
         <v>311</v>
       </c>
-      <c r="M121" t="s">
+      <c r="M122" t="s">
         <v>312</v>
-      </c>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A123" t="s">
-        <v>515</v>
-      </c>
-      <c r="M123" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A124" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="M124" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A125" t="s">
+        <v>517</v>
+      </c>
+      <c r="M125" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A126" t="s">
         <v>519</v>
       </c>
-      <c r="M125" t="s">
+      <c r="M126" t="s">
         <v>520</v>
-      </c>
-    </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A127" t="s">
-        <v>550</v>
-      </c>
-      <c r="M127" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A128" t="s">
+        <v>550</v>
+      </c>
+      <c r="M128" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A129" t="s">
         <v>551</v>
       </c>
-      <c r="M128" t="s">
+      <c r="M129" t="s">
         <v>552</v>
-      </c>
-    </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A130" t="s">
-        <v>627</v>
-      </c>
-      <c r="M130" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A131" t="s">
+        <v>627</v>
+      </c>
+      <c r="M131" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A132" t="s">
         <v>629</v>
       </c>
-      <c r="M131" t="s">
+      <c r="M132" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A133" t="s">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A134" t="s">
         <v>630</v>
       </c>
-      <c r="M133" t="s">
+      <c r="M134" t="s">
         <v>631</v>
       </c>
     </row>
@@ -7521,7 +7546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445F46B3-1A86-46EF-9440-E5378C8C2CDD}">
   <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+    <sheetView topLeftCell="A47" workbookViewId="0">
       <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat:buff Assassin option. there option Assassin  is no longer killed, and Sheriff shoot missing
</commit_message>
<xml_diff>
--- a/transData.xlsx
+++ b/transData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ドキュメント\VisualStudioProject\AmongUs\ExtremeRoles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6B1ED7-CD90-4970-9C08-19B176DDE4D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA37C3CA-C57B-4C11-A388-5AED5AA354FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21600" yWindow="1740" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="718">
   <si>
     <t>English</t>
   </si>
@@ -4930,6 +4930,63 @@
     <rPh sb="8" eb="11">
       <t>ヒヒョウジ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AssassinCanKilled</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AssassinCanKilledFromCrew</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AssassinCanKilledFromNeutral</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アサシンがキルされるか</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>キル能力を持つクルー役職がアサシンをキルできるか</t>
+    <rPh sb="2" eb="4">
+      <t>ノウリョク</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ヤクショク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>キル能力を持つ第三陣営がアサシンをキルできるか</t>
+    <rPh sb="5" eb="6">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="7" eb="11">
+      <t>ダイサンジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Retaliate</t>
+  </si>
+  <si>
+    <t>返り討ち</t>
+    <rPh sb="0" eb="4">
+      <t>カエ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SheriffCanShootAssassin</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アサシンをキルできるか</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5261,10 +5318,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q134"/>
+  <dimension ref="A1:Q135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C118" workbookViewId="0">
-      <selection activeCell="M127" sqref="M127"/>
+    <sheetView topLeftCell="C97" workbookViewId="0">
+      <selection activeCell="M102" sqref="M102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -6058,201 +6115,209 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A101" t="s">
-        <v>633</v>
+        <v>714</v>
       </c>
       <c r="M101" t="s">
-        <v>635</v>
+        <v>715</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A102" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="M102" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A103" t="s">
+        <v>634</v>
+      </c>
+      <c r="M103" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A104" t="s">
         <v>650</v>
       </c>
-      <c r="M103" t="s">
+      <c r="M104" t="s">
         <v>651</v>
-      </c>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A105" t="s">
-        <v>512</v>
-      </c>
-      <c r="M105" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A106" t="s">
+        <v>512</v>
+      </c>
+      <c r="M106" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A107" t="s">
         <v>511</v>
       </c>
-      <c r="M106" t="s">
+      <c r="M107" t="s">
         <v>514</v>
-      </c>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A108" t="s">
-        <v>304</v>
-      </c>
-      <c r="M108" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A109" t="s">
+        <v>304</v>
+      </c>
+      <c r="M109" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A110" t="s">
         <v>305</v>
       </c>
-      <c r="M109" t="s">
+      <c r="M110" t="s">
         <v>385</v>
-      </c>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A111" t="s">
-        <v>409</v>
-      </c>
-      <c r="M111" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A112" t="s">
+        <v>409</v>
+      </c>
+      <c r="M112" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A113" t="s">
         <v>408</v>
       </c>
-      <c r="M112" t="s">
+      <c r="M113" t="s">
         <v>410</v>
-      </c>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A114" t="s">
-        <v>239</v>
-      </c>
-      <c r="M114" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A115" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="M115" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A116" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="M116" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A117" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M117" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A118" t="s">
+        <v>242</v>
+      </c>
+      <c r="M118" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A119" t="s">
         <v>243</v>
       </c>
-      <c r="M118" t="s">
+      <c r="M119" t="s">
         <v>245</v>
-      </c>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A120" t="s">
-        <v>325</v>
-      </c>
-      <c r="M120" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A121" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="M121" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A122" t="s">
+        <v>324</v>
+      </c>
+      <c r="M122" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A123" t="s">
         <v>311</v>
       </c>
-      <c r="M122" t="s">
+      <c r="M123" t="s">
         <v>312</v>
-      </c>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A124" t="s">
-        <v>515</v>
-      </c>
-      <c r="M124" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A125" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="M125" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A126" t="s">
+        <v>517</v>
+      </c>
+      <c r="M126" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A127" t="s">
         <v>519</v>
       </c>
-      <c r="M126" t="s">
+      <c r="M127" t="s">
         <v>520</v>
-      </c>
-    </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A128" t="s">
-        <v>550</v>
-      </c>
-      <c r="M128" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A129" t="s">
+        <v>550</v>
+      </c>
+      <c r="M129" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A130" t="s">
         <v>551</v>
       </c>
-      <c r="M129" t="s">
+      <c r="M130" t="s">
         <v>552</v>
-      </c>
-    </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A131" t="s">
-        <v>627</v>
-      </c>
-      <c r="M131" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A132" t="s">
+        <v>627</v>
+      </c>
+      <c r="M132" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A133" t="s">
         <v>629</v>
       </c>
-      <c r="M132" t="s">
+      <c r="M133" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A134" t="s">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A135" t="s">
         <v>630</v>
       </c>
-      <c r="M134" t="s">
+      <c r="M135" t="s">
         <v>631</v>
       </c>
     </row>
@@ -6265,10 +6330,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5C264A-D4F8-4177-9D21-7A3435066086}">
-  <dimension ref="A1:Q58"/>
+  <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -6522,39 +6587,39 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>399</v>
+        <v>716</v>
       </c>
       <c r="M28" t="s">
-        <v>429</v>
+        <v>717</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
+        <v>399</v>
+      </c>
+      <c r="M29" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
         <v>400</v>
       </c>
-      <c r="M29" t="s">
+      <c r="M30" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
+    <row r="31" spans="1:13" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
         <v>522</v>
       </c>
-      <c r="M30" s="2" t="s">
+      <c r="M31" s="2" t="s">
         <v>558</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
-        <v>523</v>
-      </c>
-      <c r="M32" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>417</v>
+        <v>523</v>
       </c>
       <c r="M33" t="s">
         <v>428</v>
@@ -6562,95 +6627,95 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="M34" t="s">
-        <v>110</v>
+        <v>428</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="M35" t="s">
-        <v>432</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="M36" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
+        <v>420</v>
+      </c>
+      <c r="M37" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
         <v>421</v>
       </c>
-      <c r="M37" t="s">
+      <c r="M38" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="M38" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="M39" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A40" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="M39" t="s">
+      <c r="M40" t="s">
         <v>426</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A40" t="s">
-        <v>424</v>
-      </c>
-      <c r="M40" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
+        <v>424</v>
+      </c>
+      <c r="M41" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
         <v>425</v>
       </c>
-      <c r="M41" t="s">
+      <c r="M42" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="75" x14ac:dyDescent="0.4">
-      <c r="A42" t="s">
+    <row r="43" spans="1:13" ht="75" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
         <v>524</v>
       </c>
-      <c r="M42" s="2" t="s">
+      <c r="M43" s="2" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A43" t="s">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
         <v>438</v>
       </c>
-      <c r="M43" t="s">
+      <c r="M44" t="s">
         <v>439</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A45" t="s">
-        <v>495</v>
-      </c>
-      <c r="M45" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="M46" t="s">
         <v>496</v>
@@ -6658,97 +6723,105 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="M47" t="s">
-        <v>110</v>
+        <v>496</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="M48" t="s">
-        <v>432</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="M49" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
+        <v>500</v>
+      </c>
+      <c r="M50" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A51" t="s">
         <v>501</v>
       </c>
-      <c r="M50" t="s">
+      <c r="M51" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A51" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="M51" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="M52" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A53" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="M52" t="s">
+      <c r="M53" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A53" t="s">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A54" t="s">
         <v>624</v>
       </c>
-      <c r="M53" t="s">
+      <c r="M54" t="s">
         <v>625</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A54" s="1" t="s">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A55" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="M54" t="s">
+      <c r="M55" t="s">
         <v>626</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A55" t="s">
-        <v>502</v>
-      </c>
-      <c r="M55" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
+        <v>502</v>
+      </c>
+      <c r="M56" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A57" t="s">
         <v>503</v>
       </c>
-      <c r="M56" t="s">
+      <c r="M57" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A57" t="s">
+    <row r="58" spans="1:13" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A58" t="s">
         <v>526</v>
       </c>
-      <c r="M57" s="2" t="s">
+      <c r="M58" s="2" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A58" t="s">
+    <row r="59" spans="1:13" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
         <v>535</v>
       </c>
-      <c r="M58" s="2" t="s">
+      <c r="M59" s="2" t="s">
         <v>536</v>
       </c>
     </row>
@@ -7546,7 +7619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445F46B3-1A86-46EF-9440-E5378C8C2CDD}">
   <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
@@ -8055,10 +8128,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA3747E3-550F-4585-A066-931F491B69D2}">
-  <dimension ref="A1:Q77"/>
+  <dimension ref="A1:Q80"/>
   <sheetViews>
-    <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -8215,383 +8288,383 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>157</v>
+        <v>708</v>
       </c>
       <c r="M14" t="s">
-        <v>158</v>
+        <v>711</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>159</v>
+        <v>709</v>
       </c>
       <c r="M15" t="s">
-        <v>160</v>
+        <v>712</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>161</v>
+        <v>710</v>
       </c>
       <c r="M16" t="s">
-        <v>435</v>
+        <v>713</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="M17" t="s">
-        <v>434</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="M18" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="M19" t="s">
-        <v>168</v>
+        <v>435</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="M20" t="s">
-        <v>169</v>
+        <v>434</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="M21" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>371</v>
+        <v>165</v>
       </c>
       <c r="M22" t="s">
-        <v>372</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>212</v>
+        <v>166</v>
       </c>
       <c r="M23" t="s">
-        <v>223</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>213</v>
+        <v>167</v>
       </c>
       <c r="M24" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="111.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>537</v>
-      </c>
-      <c r="M25" s="2" t="s">
-        <v>648</v>
+        <v>371</v>
+      </c>
+      <c r="M25" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="M26" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="M27" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="273.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="111.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>313</v>
+        <v>215</v>
       </c>
       <c r="M29" t="s">
-        <v>622</v>
+        <v>218</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>315</v>
+        <v>216</v>
       </c>
       <c r="M30" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="262.5" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>314</v>
-      </c>
-      <c r="M31" t="s">
-        <v>317</v>
+        <v>538</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>313</v>
+      </c>
+      <c r="M32" t="s">
+        <v>622</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>235</v>
+        <v>315</v>
       </c>
       <c r="M33" t="s">
-        <v>174</v>
+        <v>316</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>171</v>
+        <v>314</v>
       </c>
       <c r="M34" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
-        <v>172</v>
-      </c>
-      <c r="M35" t="s">
-        <v>175</v>
+        <v>317</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>173</v>
+        <v>235</v>
       </c>
       <c r="M36" t="s">
-        <v>141</v>
+        <v>174</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="M37" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="M38" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="M39" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="M40" t="s">
-        <v>432</v>
+        <v>179</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="M41" t="s">
-        <v>433</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="M42" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="M43" t="s">
-        <v>185</v>
+        <v>432</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="M44" t="s">
-        <v>187</v>
+        <v>433</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="M45" t="s">
-        <v>193</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="M46" t="s">
-        <v>123</v>
+        <v>185</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="M47" t="s">
-        <v>122</v>
+        <v>187</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M48" t="s">
-        <v>124</v>
+        <v>193</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="M49" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>219</v>
+        <v>190</v>
       </c>
       <c r="M50" t="s">
-        <v>224</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
+        <v>191</v>
+      </c>
+      <c r="M51" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A52" t="s">
+        <v>192</v>
+      </c>
+      <c r="M52" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A53" t="s">
+        <v>219</v>
+      </c>
+      <c r="M53" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A54" t="s">
         <v>220</v>
       </c>
-      <c r="M51" t="s">
+      <c r="M54" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="280.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A52" t="s">
+    <row r="55" spans="1:13" ht="284.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A55" t="s">
         <v>539</v>
       </c>
-      <c r="M52" s="2" t="s">
+      <c r="M55" s="2" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="243.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A53" t="s">
+    <row r="56" spans="1:13" ht="243.75" x14ac:dyDescent="0.4">
+      <c r="A56" t="s">
         <v>541</v>
       </c>
-      <c r="M53" s="2" t="s">
+      <c r="M56" s="2" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="154.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A54" t="s">
+    <row r="57" spans="1:13" ht="150" x14ac:dyDescent="0.4">
+      <c r="A57" t="s">
         <v>540</v>
       </c>
-      <c r="M54" s="2" t="s">
+      <c r="M57" s="2" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A55" t="s">
+    <row r="58" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A58" t="s">
         <v>542</v>
       </c>
-      <c r="M55" s="2" t="s">
+      <c r="M58" s="2" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A56" t="s">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
         <v>493</v>
       </c>
-      <c r="M56" t="s">
+      <c r="M59" t="s">
         <v>494</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A57" t="s">
-        <v>548</v>
-      </c>
-      <c r="M57" s="2" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A58" t="s">
-        <v>369</v>
-      </c>
-      <c r="M58" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
-        <v>471</v>
-      </c>
-      <c r="M60" t="s">
-        <v>472</v>
+        <v>548</v>
+      </c>
+      <c r="M60" s="2" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
-        <v>473</v>
+        <v>369</v>
       </c>
       <c r="M61" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A62" t="s">
-        <v>474</v>
-      </c>
-      <c r="M62" t="s">
-        <v>475</v>
+        <v>370</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="M63" t="s">
         <v>472</v>
@@ -8599,113 +8672,137 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="M64" t="s">
-        <v>141</v>
+        <v>476</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="M65" t="s">
-        <v>179</v>
+        <v>475</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="M66" t="s">
-        <v>180</v>
+        <v>472</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="M67" t="s">
-        <v>432</v>
+        <v>141</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="M68" t="s">
-        <v>433</v>
+        <v>179</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="M69" t="s">
-        <v>111</v>
+        <v>180</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="M70" t="s">
-        <v>123</v>
+        <v>432</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="M71" t="s">
-        <v>122</v>
+        <v>433</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="M72" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="M73" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="M74" t="s">
-        <v>490</v>
+        <v>122</v>
       </c>
     </row>
     <row r="75" spans="1:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
+        <v>486</v>
+      </c>
+      <c r="M75" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A76" t="s">
+        <v>487</v>
+      </c>
+      <c r="M76" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A77" t="s">
+        <v>488</v>
+      </c>
+      <c r="M77" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A78" t="s">
         <v>489</v>
       </c>
-      <c r="M75" t="s">
+      <c r="M78" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="170.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A76" t="s">
+    <row r="79" spans="1:13" ht="168.75" x14ac:dyDescent="0.4">
+      <c r="A79" t="s">
         <v>543</v>
       </c>
-      <c r="M76" s="2" t="s">
+      <c r="M79" s="2" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="168.75" x14ac:dyDescent="0.4">
-      <c r="A77" t="s">
+    <row r="80" spans="1:13" ht="168.75" x14ac:dyDescent="0.4">
+      <c r="A80" t="s">
         <v>544</v>
       </c>
-      <c r="M77" s="2" t="s">
+      <c r="M80" s="2" t="s">
         <v>620</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat:new option vent player kill
</commit_message>
<xml_diff>
--- a/transData.xlsx
+++ b/transData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ドキュメント\VisualStudioProject\AmongUs\ExtremeRoles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9FAD6DC-C31E-4229-AA95-8B5EFDBBE094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54857D93-8459-4635-B22A-A5AED55DF3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="754">
   <si>
     <t>English</t>
   </si>
@@ -199,9 +199,6 @@
   </si>
   <si>
     <t>Allow Parallel MedBay Scans</t>
-  </si>
-  <si>
-    <t>メッドベイスキャン同時使用可</t>
   </si>
   <si>
     <t>Total Meetings</t>
@@ -5269,6 +5266,20 @@
     <rPh sb="7" eb="9">
       <t>カクニン</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CanKillVentInPlayer</t>
+  </si>
+  <si>
+    <t>ベント内のプレイヤーをキルできるか</t>
+    <rPh sb="3" eb="4">
+      <t>ナイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メッドベイのスキャンを同時使用できるか</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5600,10 +5611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q142"/>
+  <dimension ref="A1:Q143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="B140" sqref="B140"/>
+    <sheetView tabSelected="1" topLeftCell="D15" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -5665,7 +5676,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
@@ -5742,10 +5753,10 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="M10" t="s">
         <v>283</v>
-      </c>
-      <c r="M10" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.4">
@@ -5756,7 +5767,7 @@
         <v>33</v>
       </c>
       <c r="M11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.4">
@@ -5767,7 +5778,7 @@
         <v>34</v>
       </c>
       <c r="M12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.4">
@@ -5778,7 +5789,7 @@
         <v>35</v>
       </c>
       <c r="M13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.4">
@@ -5789,7 +5800,7 @@
         <v>36</v>
       </c>
       <c r="M14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.4">
@@ -5800,7 +5811,7 @@
         <v>37</v>
       </c>
       <c r="M15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.4">
@@ -5811,31 +5822,31 @@
         <v>38</v>
       </c>
       <c r="M16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="M19" t="s">
         <v>270</v>
-      </c>
-      <c r="M19" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B20" t="s">
         <v>48</v>
@@ -5846,18 +5857,18 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
         <v>50</v>
       </c>
       <c r="M21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" t="s">
         <v>51</v>
@@ -5868,40 +5879,40 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
         <v>53</v>
       </c>
       <c r="M23" t="s">
-        <v>54</v>
+        <v>753</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="M25" t="s">
         <v>274</v>
       </c>
-      <c r="M25" t="s">
-        <v>275</v>
-      </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A26" s="1" t="s">
-        <v>273</v>
+      <c r="A26" t="s">
+        <v>751</v>
       </c>
       <c r="M26" t="s">
-        <v>276</v>
+        <v>752</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.4">
@@ -5909,50 +5920,47 @@
         <v>272</v>
       </c>
       <c r="M27" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A29" t="s">
-        <v>278</v>
-      </c>
-      <c r="M29" t="s">
-        <v>280</v>
+        <v>275</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A28" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="M28" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
+        <v>277</v>
+      </c>
+      <c r="M30" t="s">
         <v>279</v>
-      </c>
-      <c r="M30" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="M31" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32" t="s">
-        <v>62</v>
+        <v>280</v>
       </c>
       <c r="M32" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="M33" t="s">
         <v>298</v>
@@ -5960,10 +5968,10 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M34" t="s">
         <v>297</v>
@@ -5971,10 +5979,10 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M35" t="s">
         <v>296</v>
@@ -5982,104 +5990,104 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" t="s">
+        <v>67</v>
+      </c>
+      <c r="M36" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
+        <v>698</v>
+      </c>
+      <c r="B37" t="s">
         <v>699</v>
       </c>
-      <c r="B36" t="s">
+      <c r="M37" t="s">
         <v>700</v>
       </c>
-      <c r="M36" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A38" t="s">
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>438</v>
+      </c>
+      <c r="M39" t="s">
         <v>439</v>
-      </c>
-      <c r="M38" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A40" t="s">
-        <v>286</v>
-      </c>
-      <c r="M40" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="M41" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="M42" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="M43" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A45" t="s">
-        <v>287</v>
-      </c>
-      <c r="M45" t="s">
-        <v>441</v>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
+        <v>290</v>
+      </c>
+      <c r="M44" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="M46" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="M47" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
+        <v>291</v>
+      </c>
+      <c r="M48" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
+        <v>292</v>
+      </c>
+      <c r="M49" t="s">
         <v>293</v>
-      </c>
-      <c r="M48" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A50" t="s">
-        <v>631</v>
-      </c>
-      <c r="B50" t="s">
-        <v>638</v>
-      </c>
-      <c r="M50" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B51" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
       <c r="M51" t="s">
         <v>636</v>
@@ -6087,108 +6095,108 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
-        <v>634</v>
+        <v>631</v>
+      </c>
+      <c r="B52" t="s">
+        <v>632</v>
       </c>
       <c r="M52" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A58" t="s">
-        <v>412</v>
-      </c>
-      <c r="M58" t="s">
-        <v>300</v>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A53" t="s">
+        <v>633</v>
+      </c>
+      <c r="M53" t="s">
+        <v>634</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="M59" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="M60" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A62" t="s">
-        <v>69</v>
-      </c>
-      <c r="B62" t="s">
-        <v>70</v>
-      </c>
-      <c r="M62" t="s">
-        <v>71</v>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A61" t="s">
+        <v>410</v>
+      </c>
+      <c r="M61" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
+        <v>68</v>
+      </c>
+      <c r="B63" t="s">
+        <v>69</v>
+      </c>
+      <c r="M63" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A64" t="s">
+        <v>71</v>
+      </c>
+      <c r="B64" t="s">
         <v>72</v>
       </c>
-      <c r="B63" t="s">
+      <c r="M64" t="s">
         <v>73</v>
-      </c>
-      <c r="M63" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A65" t="s">
-        <v>97</v>
-      </c>
-      <c r="B65" t="s">
-        <v>98</v>
-      </c>
-      <c r="M65" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B66" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="M66" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B67" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="M67" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A69" t="s">
-        <v>76</v>
-      </c>
-      <c r="B69" t="s">
-        <v>77</v>
-      </c>
-      <c r="M69" t="s">
-        <v>86</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A68" t="s">
+        <v>95</v>
+      </c>
+      <c r="B68" t="s">
+        <v>99</v>
+      </c>
+      <c r="M68" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B70" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M70" t="s">
         <v>85</v>
@@ -6196,98 +6204,98 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
+        <v>77</v>
+      </c>
+      <c r="B71" t="s">
+        <v>78</v>
+      </c>
+      <c r="M71" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A72" t="s">
+        <v>79</v>
+      </c>
+      <c r="B72" t="s">
         <v>80</v>
       </c>
-      <c r="B71" t="s">
+      <c r="M72" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A74" t="s">
         <v>81</v>
       </c>
-      <c r="M71" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A73" t="s">
+      <c r="B74" t="s">
         <v>82</v>
       </c>
-      <c r="B73" t="s">
+      <c r="M74" t="s">
         <v>83</v>
-      </c>
-      <c r="M73" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A75" t="s">
-        <v>246</v>
-      </c>
-      <c r="B75" t="s">
-        <v>247</v>
-      </c>
-      <c r="M75" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
+        <v>245</v>
+      </c>
+      <c r="B76" t="s">
+        <v>246</v>
+      </c>
+      <c r="M76" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A77" t="s">
+        <v>247</v>
+      </c>
+      <c r="B77" t="s">
         <v>248</v>
       </c>
-      <c r="B76" t="s">
+      <c r="M77" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A79" t="s">
         <v>249</v>
       </c>
-      <c r="M76" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A78" t="s">
+      <c r="B79" t="s">
         <v>250</v>
       </c>
-      <c r="B78" t="s">
+      <c r="M79" t="s">
         <v>251</v>
-      </c>
-      <c r="M78" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A80" t="s">
-        <v>253</v>
-      </c>
-      <c r="B80" t="s">
-        <v>254</v>
-      </c>
-      <c r="M80" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B81" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="M81" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
-        <v>303</v>
+        <v>255</v>
       </c>
       <c r="B82" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="M82" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
-        <v>260</v>
+        <v>302</v>
       </c>
       <c r="B83" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="M83" t="s">
         <v>264</v>
@@ -6295,77 +6303,80 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
-        <v>328</v>
+        <v>259</v>
       </c>
       <c r="B84" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="M84" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
+        <v>327</v>
+      </c>
+      <c r="B85" t="s">
+        <v>260</v>
+      </c>
+      <c r="M85" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A86" t="s">
+        <v>328</v>
+      </c>
+      <c r="B86" t="s">
         <v>329</v>
       </c>
-      <c r="B85" t="s">
-        <v>330</v>
-      </c>
-      <c r="M85" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A88" t="s">
+      <c r="M86" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A89" t="s">
+        <v>306</v>
+      </c>
+      <c r="M89" t="s">
         <v>307</v>
-      </c>
-      <c r="M88" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A90" t="s">
-        <v>385</v>
-      </c>
-      <c r="M90" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="M91" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A94" t="s">
-        <v>372</v>
-      </c>
-      <c r="M94" t="s">
-        <v>382</v>
+        <v>385</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A92" t="s">
+        <v>386</v>
+      </c>
+      <c r="M92" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A95" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="M95" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A96" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="M96" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A97" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="M97" t="s">
         <v>380</v>
@@ -6373,7 +6384,7 @@
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="M98" t="s">
         <v>379</v>
@@ -6381,7 +6392,7 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="M99" t="s">
         <v>378</v>
@@ -6389,50 +6400,50 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A100" t="s">
-        <v>413</v>
+        <v>376</v>
       </c>
       <c r="M100" t="s">
-        <v>414</v>
+        <v>377</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A101" t="s">
-        <v>708</v>
+        <v>412</v>
       </c>
       <c r="M101" t="s">
-        <v>709</v>
+        <v>413</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A102" t="s">
-        <v>627</v>
+        <v>707</v>
       </c>
       <c r="M102" t="s">
-        <v>629</v>
+        <v>708</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A103" t="s">
+        <v>626</v>
+      </c>
+      <c r="M103" t="s">
         <v>628</v>
-      </c>
-      <c r="M103" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A104" t="s">
+        <v>627</v>
+      </c>
+      <c r="M104" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A105" t="s">
+        <v>643</v>
+      </c>
+      <c r="M105" t="s">
         <v>644</v>
-      </c>
-      <c r="M104" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A106" t="s">
-        <v>511</v>
-      </c>
-      <c r="M106" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.4">
@@ -6440,31 +6451,31 @@
         <v>510</v>
       </c>
       <c r="M107" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A109" t="s">
-        <v>304</v>
-      </c>
-      <c r="M109" t="s">
-        <v>306</v>
+        <v>511</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A108" t="s">
+        <v>509</v>
+      </c>
+      <c r="M108" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A110" t="s">
+        <v>303</v>
+      </c>
+      <c r="M110" t="s">
         <v>305</v>
       </c>
-      <c r="M110" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A112" t="s">
-        <v>408</v>
-      </c>
-      <c r="M112" t="s">
-        <v>406</v>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A111" t="s">
+        <v>304</v>
+      </c>
+      <c r="M111" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.4">
@@ -6472,15 +6483,15 @@
         <v>407</v>
       </c>
       <c r="M113" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A115" t="s">
-        <v>239</v>
-      </c>
-      <c r="M115" t="s">
-        <v>236</v>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A114" t="s">
+        <v>406</v>
+      </c>
+      <c r="M114" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.4">
@@ -6488,39 +6499,39 @@
         <v>238</v>
       </c>
       <c r="M116" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A117" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="M117" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A118" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="M118" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A119" t="s">
+        <v>241</v>
+      </c>
+      <c r="M119" t="s">
         <v>243</v>
       </c>
-      <c r="M119" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A121" t="s">
-        <v>324</v>
-      </c>
-      <c r="M121" t="s">
-        <v>331</v>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A120" t="s">
+        <v>242</v>
+      </c>
+      <c r="M120" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.4">
@@ -6528,127 +6539,135 @@
         <v>323</v>
       </c>
       <c r="M122" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A123" t="s">
+        <v>322</v>
+      </c>
+      <c r="M123" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A124" t="s">
+        <v>310</v>
+      </c>
+      <c r="M124" t="s">
         <v>311</v>
-      </c>
-      <c r="M123" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A125" t="s">
-        <v>514</v>
-      </c>
-      <c r="M125" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A126" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="M126" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A127" t="s">
+        <v>515</v>
+      </c>
+      <c r="M127" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A128" t="s">
+        <v>517</v>
+      </c>
+      <c r="M128" t="s">
         <v>518</v>
-      </c>
-      <c r="M127" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A129" t="s">
-        <v>548</v>
-      </c>
-      <c r="M129" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A130" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="M130" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A132" t="s">
-        <v>621</v>
-      </c>
-      <c r="M132" t="s">
-        <v>622</v>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A131" t="s">
+        <v>548</v>
+      </c>
+      <c r="M131" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A133" t="s">
+        <v>620</v>
+      </c>
+      <c r="M133" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A134" t="s">
+        <v>622</v>
+      </c>
+      <c r="M134" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A136" t="s">
         <v>623</v>
       </c>
-      <c r="M133" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A135" t="s">
+      <c r="M136" t="s">
         <v>624</v>
-      </c>
-      <c r="M135" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A137" t="s">
-        <v>740</v>
-      </c>
-      <c r="M137" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A138" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="M138" t="s">
-        <v>742</v>
+        <v>750</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A139" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="M139" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A140" t="s">
+        <v>742</v>
+      </c>
+      <c r="M140" t="s">
         <v>744</v>
-      </c>
-      <c r="M140" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A141" t="s">
-        <v>748</v>
+        <v>743</v>
       </c>
       <c r="M141" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A142" t="s">
+        <v>747</v>
+      </c>
+      <c r="M142" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A143" t="s">
+        <v>748</v>
+      </c>
+      <c r="M143" t="s">
         <v>749</v>
-      </c>
-      <c r="M142" t="s">
-        <v>750</v>
       </c>
     </row>
   </sheetData>
@@ -6724,436 +6743,436 @@
     </row>
     <row r="2" spans="1:17" ht="39" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="M3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="57" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="41.25" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
+        <v>107</v>
+      </c>
+      <c r="M7" t="s">
         <v>108</v>
-      </c>
-      <c r="M7" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M10" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
+        <v>194</v>
+      </c>
+      <c r="M13" t="s">
         <v>195</v>
-      </c>
-      <c r="M13" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="39" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="M16" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="M17" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="M18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="M19" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="M20" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="M21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="M22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="M23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="M25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="M26" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="M27" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
+        <v>709</v>
+      </c>
+      <c r="M28" t="s">
         <v>710</v>
-      </c>
-      <c r="M28" t="s">
-        <v>711</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="M29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="M30" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="111" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="33" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="M33" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="M34" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="M35" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="M36" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="M37" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="M38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="M39" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="M40" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="M41" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="M42" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="75" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
+        <v>436</v>
+      </c>
+      <c r="M44" t="s">
         <v>437</v>
-      </c>
-      <c r="M44" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
+        <v>493</v>
+      </c>
+      <c r="M46" t="s">
         <v>494</v>
-      </c>
-      <c r="M46" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="M47" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="M48" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="M49" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="M50" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="M51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="M52" t="s">
         <v>503</v>
-      </c>
-      <c r="M52" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A53" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="M53" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
+        <v>617</v>
+      </c>
+      <c r="M54" t="s">
         <v>618</v>
-      </c>
-      <c r="M54" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A55" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="M55" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="M56" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="M57" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
+        <v>524</v>
+      </c>
+      <c r="M58" s="2" t="s">
         <v>525</v>
-      </c>
-      <c r="M58" s="2" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
+        <v>532</v>
+      </c>
+      <c r="M59" s="2" t="s">
         <v>533</v>
-      </c>
-      <c r="M59" s="2" t="s">
-        <v>534</v>
       </c>
     </row>
   </sheetData>
@@ -7229,714 +7248,714 @@
     </row>
     <row r="2" spans="1:17" ht="54.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>560</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>561</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="92.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>562</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>563</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M8" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M9" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="64.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="M15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
+        <v>345</v>
+      </c>
+      <c r="M19" t="s">
         <v>346</v>
-      </c>
-      <c r="M19" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="M20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="M21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="M22" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="M23" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="M24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="M25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="M26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="M27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="M28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="M29" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="M30" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="M31" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="M32" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="M33" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="M34" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="M35" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="83.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M36" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="M37" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
+        <v>355</v>
+      </c>
+      <c r="M38" t="s">
         <v>356</v>
-      </c>
-      <c r="M38" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="75" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="M40" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
+        <v>359</v>
+      </c>
+      <c r="M41" t="s">
         <v>360</v>
-      </c>
-      <c r="M41" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="M43" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="M44" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="M45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A46" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="M46" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="M47" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="M48" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="M49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="M50" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A51" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="M51" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="M52" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A53" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="M53" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A54" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="M54" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A55" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="M55" t="s">
         <v>468</v>
-      </c>
-      <c r="M55" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="M56" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="M57" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
+        <v>528</v>
+      </c>
+      <c r="M58" s="2" t="s">
         <v>529</v>
-      </c>
-      <c r="M58" s="2" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
+        <v>461</v>
+      </c>
+      <c r="M59" t="s">
         <v>462</v>
-      </c>
-      <c r="M59" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
+        <v>575</v>
+      </c>
+      <c r="M61" t="s">
         <v>576</v>
-      </c>
-      <c r="M61" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A62" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="M62" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A63" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="M63" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A64" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="M64" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A65" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="M65" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A66" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="M66" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A67" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="M67" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A68" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="M68" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A69" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="M69" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A70" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="M70" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A71" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="M71" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A72" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="M72" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A73" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="M73" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="M74" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="M75" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="76" spans="1:13" ht="135.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="M76" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="M78" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A79" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="M79" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="M80" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A81" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="M81" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A82" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="M82" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A83" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="M83" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A84" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="M84" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A85" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="M85" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A86" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="M86" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A87" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="M87" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A88" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="M88" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A89" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="M89" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A90" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="M90" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A91" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="M91" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A92" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="M92" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="M93" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="M94" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="95" spans="1:13" ht="96" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A95" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="M95" s="2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
   </sheetData>
@@ -8012,538 +8031,538 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
+        <v>308</v>
+      </c>
+      <c r="M13" t="s">
         <v>309</v>
-      </c>
-      <c r="M13" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="M14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M15" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M16" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="177" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
+        <v>325</v>
+      </c>
+      <c r="M20" t="s">
         <v>326</v>
-      </c>
-      <c r="M20" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
+        <v>227</v>
+      </c>
+      <c r="M22" t="s">
         <v>228</v>
-      </c>
-      <c r="M22" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="M23" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
+        <v>137</v>
+      </c>
+      <c r="M24" t="s">
         <v>138</v>
-      </c>
-      <c r="M24" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A46" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M52" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M53" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="131.25" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
+        <v>543</v>
+      </c>
+      <c r="M55" t="s">
         <v>544</v>
-      </c>
-      <c r="M55" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
+        <v>207</v>
+      </c>
+      <c r="M56" t="s">
         <v>208</v>
-      </c>
-      <c r="M56" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="75" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A59" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="M59" t="s">
         <v>719</v>
-      </c>
-      <c r="M59" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A60" s="1" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="M60" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A61" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A62" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A63" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A64" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A65" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A66" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A67" s="1" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="M67" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="M68" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="M69" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="70" spans="1:13" ht="95.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="M70" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
   </sheetData>
@@ -8619,618 +8638,618 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>231</v>
+      </c>
+      <c r="M3" t="s">
         <v>232</v>
-      </c>
-      <c r="M3" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M7" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M8" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
+        <v>149</v>
+      </c>
+      <c r="M11" t="s">
         <v>150</v>
-      </c>
-      <c r="M11" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="M14" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="M15" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="M16" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
+        <v>156</v>
+      </c>
+      <c r="M17" t="s">
         <v>157</v>
-      </c>
-      <c r="M17" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
+        <v>158</v>
+      </c>
+      <c r="M18" t="s">
         <v>159</v>
-      </c>
-      <c r="M18" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M19" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="M20" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
+        <v>162</v>
+      </c>
+      <c r="M21" t="s">
         <v>163</v>
-      </c>
-      <c r="M21" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
+        <v>369</v>
+      </c>
+      <c r="M25" t="s">
         <v>370</v>
-      </c>
-      <c r="M25" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
+        <v>212</v>
+      </c>
+      <c r="M27" t="s">
         <v>213</v>
-      </c>
-      <c r="M27" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="111.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="M29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
+        <v>215</v>
+      </c>
+      <c r="M30" t="s">
         <v>216</v>
-      </c>
-      <c r="M30" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="262.5" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M32" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
+        <v>314</v>
+      </c>
+      <c r="M33" t="s">
         <v>315</v>
-      </c>
-      <c r="M33" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="M34" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M38" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M42" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M43" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M44" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
+        <v>183</v>
+      </c>
+      <c r="M46" t="s">
         <v>184</v>
-      </c>
-      <c r="M46" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
+        <v>185</v>
+      </c>
+      <c r="M47" t="s">
         <v>186</v>
-      </c>
-      <c r="M47" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M48" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M50" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M51" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M52" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M53" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
+        <v>219</v>
+      </c>
+      <c r="M54" t="s">
         <v>220</v>
-      </c>
-      <c r="M54" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="284.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="56" spans="1:13" ht="243.75" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="150" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
+        <v>491</v>
+      </c>
+      <c r="M59" t="s">
         <v>492</v>
-      </c>
-      <c r="M59" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
+        <v>545</v>
+      </c>
+      <c r="M60" s="2" t="s">
         <v>546</v>
-      </c>
-      <c r="M60" s="2" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
+        <v>367</v>
+      </c>
+      <c r="M61" t="s">
         <v>368</v>
-      </c>
-      <c r="M61" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
+        <v>469</v>
+      </c>
+      <c r="M63" t="s">
         <v>470</v>
-      </c>
-      <c r="M63" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="M64" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
+        <v>472</v>
+      </c>
+      <c r="M65" t="s">
         <v>473</v>
-      </c>
-      <c r="M65" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="M66" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="M67" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="M68" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M69" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="M70" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="M71" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="M72" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="M73" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="M74" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="75" spans="1:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="M75" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="76" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="M76" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="M77" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="M78" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="79" spans="1:13" ht="168.75" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="M79" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="80" spans="1:13" ht="168.75" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="M80" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change:role name admin to supervisor
</commit_message>
<xml_diff>
--- a/transData.xlsx
+++ b/transData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ドキュメント\VisualStudioProject\AmongUs\ExtremeRoles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACDCAD9E-004B-44DB-B583-DC08A1611F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC18E78-69F8-4F7D-A026-A61ABFB501E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="779">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="794">
   <si>
     <t>English</t>
   </si>
@@ -5475,6 +5475,158 @@
   </si>
   <si>
     <t>船員達を監視して、怪しい奴を見つけ出せ</t>
+  </si>
+  <si>
+    <t>アドミンの使用時間</t>
+    <rPh sb="5" eb="7">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ジカン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アドミン</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Supervisor</t>
+  </si>
+  <si>
+    <t>SupervisorSpawnRate</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SupervisorRoleNum</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SupervisorHasOtherVison</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SupervisorVison</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SupervisorApplyEnvironmentVisionEffect</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SupervisorAbilityCoolTime</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SupervisorAbilityActiveTime</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スーパーバイザー</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Admin</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「アドミン」がいつでも使えるクルー役職
+使用には時間制限があり、使用する毎に時間制限は短くなる
+時間制限はクールタイムが終了するか、タスクを終了させる
+ことで役職に設定された充電の持続時間まで回復する</t>
+    <rPh sb="11" eb="12">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ジカン</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>セイゲン</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>ゴト</t>
+    </rPh>
+    <rPh sb="38" eb="42">
+      <t>ジカンセイ</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>ミジカ</t>
+    </rPh>
+    <rPh sb="48" eb="52">
+      <t>ジカンセイゲン</t>
+    </rPh>
+    <rPh sb="60" eb="62">
+      <t>シュウリョウ</t>
+    </rPh>
+    <rPh sb="70" eb="72">
+      <t>シュウリョウ</t>
+    </rPh>
+    <rPh sb="79" eb="81">
+      <t>ヤクショク</t>
+    </rPh>
+    <rPh sb="82" eb="84">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="87" eb="89">
+      <t>ジュウデン</t>
+    </rPh>
+    <rPh sb="90" eb="92">
+      <t>ジゾク</t>
+    </rPh>
+    <rPh sb="92" eb="94">
+      <t>ジカン</t>
+    </rPh>
+    <rPh sb="96" eb="98">
+      <t>カイフク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>監督者として、船員達の位置情報を収集せよ</t>
+    <rPh sb="0" eb="2">
+      <t>カントク</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>シャ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>イチ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>シュウシュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アドミンで、船員達の位置情報を洗い出せ</t>
+    <rPh sb="6" eb="8">
+      <t>センイン</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>タチ</t>
+    </rPh>
+    <rPh sb="10" eb="14">
+      <t>イチジョウホウ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>アラ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ダ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -6881,10 +7033,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5C264A-D4F8-4177-9D21-7A3435066086}">
-  <dimension ref="A1:Q73"/>
+  <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -7479,6 +7631,102 @@
       </c>
       <c r="M73" t="s">
         <v>776</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A75" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="M75" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A76" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="M76" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A77" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="M77" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A78" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="M78" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A79" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="M79" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A80" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="M80" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A81" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="M81" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A82" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="M82" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A83" t="s">
+        <v>769</v>
+      </c>
+      <c r="M83" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A84" t="s">
+        <v>770</v>
+      </c>
+      <c r="M84" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" ht="75" x14ac:dyDescent="0.4">
+      <c r="A85" t="s">
+        <v>771</v>
+      </c>
+      <c r="M85" s="2" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A86" t="s">
+        <v>790</v>
+      </c>
+      <c r="M86" s="2" t="s">
+        <v>780</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat:new option marin can't see Assassin
</commit_message>
<xml_diff>
--- a/transData.xlsx
+++ b/transData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ドキュメント\VisualStudioProject\AmongUs\ExtremeRoles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972AC0D0-7D00-4C50-A8FC-0D515C6AF9D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC09E10-C317-46FA-84F3-A2B6AA9D233A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="824">
   <si>
     <t>English</t>
   </si>
@@ -5808,6 +5808,17 @@
   </si>
   <si>
     <t>securityCamera</t>
+  </si>
+  <si>
+    <t>MarlinCanSeeAssassin</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>マーリンがアサシンを見ることができるか</t>
+    <rPh sb="10" eb="11">
+      <t>ミ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -7216,7 +7227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5C264A-D4F8-4177-9D21-7A3435066086}">
   <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+    <sheetView topLeftCell="A74" workbookViewId="0">
       <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
@@ -9453,10 +9464,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA3747E3-550F-4585-A066-931F491B69D2}">
-  <dimension ref="A1:Q80"/>
+  <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -9685,111 +9696,111 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>165</v>
+        <v>822</v>
       </c>
       <c r="M23" t="s">
-        <v>168</v>
+        <v>823</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>367</v>
+        <v>166</v>
       </c>
       <c r="M25" t="s">
-        <v>368</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>211</v>
+        <v>367</v>
       </c>
       <c r="M26" t="s">
-        <v>222</v>
+        <v>368</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M27" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="111.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
+        <v>212</v>
+      </c>
+      <c r="M28" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="112.5" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
         <v>532</v>
       </c>
-      <c r="M28" s="2" t="s">
+      <c r="M29" s="2" t="s">
         <v>639</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A29" t="s">
-        <v>214</v>
-      </c>
-      <c r="M29" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="M30" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="309" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
+        <v>215</v>
+      </c>
+      <c r="M31" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="300" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
         <v>533</v>
       </c>
-      <c r="M31" s="2" t="s">
+      <c r="M32" s="2" t="s">
         <v>757</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
-        <v>312</v>
-      </c>
-      <c r="M32" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M33" t="s">
-        <v>315</v>
+        <v>613</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
+        <v>314</v>
+      </c>
+      <c r="M34" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
         <v>313</v>
       </c>
-      <c r="M34" t="s">
+      <c r="M35" t="s">
         <v>316</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A36" t="s">
-        <v>234</v>
-      </c>
-      <c r="M36" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>170</v>
+        <v>234</v>
       </c>
       <c r="M37" t="s">
         <v>173</v>
@@ -9797,337 +9808,345 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M39" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="M40" t="s">
-        <v>178</v>
+        <v>140</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M41" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M42" t="s">
-        <v>144</v>
+        <v>179</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="M43" t="s">
-        <v>428</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M44" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M45" t="s">
-        <v>110</v>
+        <v>429</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M46" t="s">
-        <v>184</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="M47" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="M48" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M49" t="s">
-        <v>122</v>
+        <v>192</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M50" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M51" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M52" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
-        <v>218</v>
+        <v>191</v>
       </c>
       <c r="M53" t="s">
-        <v>223</v>
+        <v>124</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M54" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="284.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
+        <v>219</v>
+      </c>
+      <c r="M55" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="281.25" x14ac:dyDescent="0.4">
+      <c r="A56" t="s">
         <v>534</v>
       </c>
-      <c r="M55" s="2" t="s">
+      <c r="M56" s="2" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="243.75" x14ac:dyDescent="0.4">
-      <c r="A56" t="s">
+    <row r="57" spans="1:13" ht="243.75" x14ac:dyDescent="0.4">
+      <c r="A57" t="s">
         <v>536</v>
       </c>
-      <c r="M56" s="2" t="s">
+      <c r="M57" s="2" t="s">
         <v>637</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" ht="150" x14ac:dyDescent="0.4">
-      <c r="A57" t="s">
-        <v>535</v>
-      </c>
-      <c r="M57" s="2" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
+        <v>535</v>
+      </c>
+      <c r="M58" s="2" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
         <v>537</v>
       </c>
-      <c r="M58" s="2" t="s">
+      <c r="M59" s="2" t="s">
         <v>638</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A59" t="s">
-        <v>489</v>
-      </c>
-      <c r="M59" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
-        <v>543</v>
-      </c>
-      <c r="M60" s="2" t="s">
-        <v>544</v>
+        <v>489</v>
+      </c>
+      <c r="M60" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
+        <v>543</v>
+      </c>
+      <c r="M61" s="2" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A62" t="s">
         <v>365</v>
       </c>
-      <c r="M61" t="s">
+      <c r="M62" t="s">
         <v>366</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A63" t="s">
-        <v>467</v>
-      </c>
-      <c r="M63" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="M64" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="M65" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="M66" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="M67" t="s">
-        <v>140</v>
+        <v>468</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="M68" t="s">
-        <v>178</v>
+        <v>140</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="M69" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="M70" t="s">
-        <v>428</v>
+        <v>179</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="M71" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M72" t="s">
-        <v>110</v>
+        <v>429</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="M73" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="M74" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="75" spans="1:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="M75" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="76" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="M76" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="M77" t="s">
-        <v>486</v>
+        <v>124</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
+        <v>484</v>
+      </c>
+      <c r="M78" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A79" t="s">
         <v>485</v>
       </c>
-      <c r="M78" t="s">
+      <c r="M79" t="s">
         <v>487</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" ht="168.75" x14ac:dyDescent="0.4">
-      <c r="A79" t="s">
-        <v>538</v>
-      </c>
-      <c r="M79" s="2" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="80" spans="1:13" ht="168.75" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
+        <v>538</v>
+      </c>
+      <c r="M80" s="2" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" ht="168.75" x14ac:dyDescent="0.4">
+      <c r="A81" t="s">
         <v>539</v>
       </c>
-      <c r="M80" s="2" t="s">
+      <c r="M81" s="2" t="s">
         <v>734</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix:multi assign intro fix
</commit_message>
<xml_diff>
--- a/transData.xlsx
+++ b/transData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ドキュメント\VisualStudioProject\AmongUs\ExtremeRoles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4AF083-E334-42E9-AD14-1A38A9AB7154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE54538-5AFF-4B71-85CA-71CE9E7EF16A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="1168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1429" uniqueCount="1170">
   <si>
     <t>English</t>
   </si>
@@ -8871,6 +8871,14 @@
     <rPh sb="11" eb="13">
       <t>ミナゴロ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>introAnd</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>そして、</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -9202,10 +9210,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q168"/>
+  <dimension ref="A1:Q169"/>
   <sheetViews>
-    <sheetView topLeftCell="C110" workbookViewId="0">
-      <selection activeCell="M130" sqref="M130"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -9782,657 +9790,665 @@
         <v>295</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A69" t="s">
-        <v>66</v>
-      </c>
-      <c r="B69" t="s">
-        <v>67</v>
-      </c>
-      <c r="M69" t="s">
-        <v>68</v>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A68" t="s">
+        <v>1168</v>
+      </c>
+      <c r="M68" t="s">
+        <v>1169</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
+        <v>66</v>
+      </c>
+      <c r="B70" t="s">
+        <v>67</v>
+      </c>
+      <c r="M70" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A71" t="s">
         <v>69</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B71" t="s">
         <v>70</v>
       </c>
-      <c r="M70" t="s">
+      <c r="M71" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A72" t="s">
-        <v>94</v>
-      </c>
-      <c r="B72" t="s">
-        <v>95</v>
-      </c>
-      <c r="M72" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B73" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M73" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
+        <v>92</v>
+      </c>
+      <c r="B74" t="s">
+        <v>96</v>
+      </c>
+      <c r="M74" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A75" t="s">
         <v>93</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B75" t="s">
         <v>97</v>
       </c>
-      <c r="M74" t="s">
+      <c r="M75" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A76" t="s">
-        <v>73</v>
-      </c>
-      <c r="B76" t="s">
-        <v>74</v>
-      </c>
-      <c r="M76" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B77" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="M77" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
+        <v>75</v>
+      </c>
+      <c r="B78" t="s">
+        <v>76</v>
+      </c>
+      <c r="M78" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A79" t="s">
         <v>77</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B79" t="s">
         <v>78</v>
       </c>
-      <c r="M78" t="s">
+      <c r="M79" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A80" t="s">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A81" t="s">
         <v>79</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B81" t="s">
         <v>80</v>
       </c>
-      <c r="M80" t="s">
+      <c r="M81" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A82" t="s">
-        <v>240</v>
-      </c>
-      <c r="B82" t="s">
-        <v>241</v>
-      </c>
-      <c r="M82" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
+        <v>240</v>
+      </c>
+      <c r="B83" t="s">
+        <v>241</v>
+      </c>
+      <c r="M83" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A84" t="s">
         <v>242</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B84" t="s">
         <v>243</v>
       </c>
-      <c r="M83" t="s">
+      <c r="M84" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A85" t="s">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A86" t="s">
         <v>244</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B86" t="s">
         <v>245</v>
       </c>
-      <c r="M85" t="s">
+      <c r="M86" t="s">
         <v>246</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A87" t="s">
-        <v>247</v>
-      </c>
-      <c r="B87" t="s">
-        <v>248</v>
-      </c>
-      <c r="M87" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A88" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B88" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="M88" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A89" t="s">
-        <v>296</v>
+        <v>250</v>
       </c>
       <c r="B89" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="M89" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A90" t="s">
-        <v>1163</v>
+        <v>296</v>
       </c>
       <c r="B90" t="s">
         <v>253</v>
       </c>
       <c r="M90" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
-        <v>318</v>
+        <v>1163</v>
       </c>
       <c r="B91" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="M91" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A92" t="s">
+        <v>318</v>
+      </c>
+      <c r="B92" t="s">
+        <v>254</v>
+      </c>
+      <c r="M92" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A93" t="s">
         <v>319</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B93" t="s">
         <v>320</v>
       </c>
-      <c r="M92" t="s">
+      <c r="M93" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A95" t="s">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A96" t="s">
         <v>300</v>
       </c>
-      <c r="M95" t="s">
+      <c r="M96" t="s">
         <v>301</v>
-      </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A97" t="s">
-        <v>373</v>
-      </c>
-      <c r="M97" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
+        <v>373</v>
+      </c>
+      <c r="M98" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A99" t="s">
         <v>375</v>
       </c>
-      <c r="M98" t="s">
+      <c r="M99" t="s">
         <v>403</v>
-      </c>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A101" t="s">
-        <v>360</v>
-      </c>
-      <c r="M101" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A102" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="M102" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A103" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="M103" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A104" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="M104" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A105" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="M105" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A106" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="M106" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A107" t="s">
-        <v>401</v>
+        <v>365</v>
       </c>
       <c r="M107" t="s">
-        <v>402</v>
+        <v>366</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A108" t="s">
-        <v>691</v>
+        <v>401</v>
       </c>
       <c r="M108" t="s">
-        <v>692</v>
+        <v>402</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A109" t="s">
-        <v>611</v>
+        <v>691</v>
       </c>
       <c r="M109" t="s">
-        <v>613</v>
+        <v>692</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A110" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="M110" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A111" t="s">
-        <v>627</v>
+        <v>612</v>
       </c>
       <c r="M111" t="s">
-        <v>628</v>
+        <v>614</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A112" t="s">
-        <v>830</v>
+        <v>627</v>
       </c>
       <c r="M112" t="s">
-        <v>831</v>
+        <v>628</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A113" t="s">
-        <v>852</v>
+        <v>830</v>
       </c>
       <c r="M113" t="s">
-        <v>853</v>
+        <v>831</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A114" t="s">
+        <v>852</v>
+      </c>
+      <c r="M114" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A115" t="s">
         <v>1154</v>
       </c>
-      <c r="M114" t="s">
+      <c r="M115" t="s">
         <v>1155</v>
-      </c>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A116" t="s">
-        <v>495</v>
-      </c>
-      <c r="M116" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A117" t="s">
+        <v>495</v>
+      </c>
+      <c r="M117" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A118" t="s">
         <v>494</v>
       </c>
-      <c r="M117" t="s">
+      <c r="M118" t="s">
         <v>497</v>
-      </c>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A119" t="s">
-        <v>297</v>
-      </c>
-      <c r="M119" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A120" t="s">
+        <v>297</v>
+      </c>
+      <c r="M120" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A121" t="s">
         <v>298</v>
       </c>
-      <c r="M120" t="s">
+      <c r="M121" t="s">
         <v>372</v>
-      </c>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A122" t="s">
-        <v>396</v>
-      </c>
-      <c r="M122" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A123" t="s">
+        <v>396</v>
+      </c>
+      <c r="M123" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A124" t="s">
         <v>395</v>
       </c>
-      <c r="M123" t="s">
+      <c r="M124" t="s">
         <v>397</v>
-      </c>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A125" t="s">
-        <v>234</v>
-      </c>
-      <c r="M125" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A126" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="M126" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A127" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="M127" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A128" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M128" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A129" t="s">
+        <v>237</v>
+      </c>
+      <c r="M129" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A130" t="s">
         <v>238</v>
       </c>
-      <c r="M129" t="s">
+      <c r="M130" t="s">
         <v>1164</v>
-      </c>
-    </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A131" t="s">
-        <v>314</v>
-      </c>
-      <c r="M131" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A132" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="M132" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A133" t="s">
+        <v>313</v>
+      </c>
+      <c r="M133" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A134" t="s">
         <v>303</v>
       </c>
-      <c r="M133" t="s">
+      <c r="M134" t="s">
         <v>304</v>
-      </c>
-    </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A135" t="s">
-        <v>498</v>
-      </c>
-      <c r="M135" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A136" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="M136" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A137" t="s">
+        <v>500</v>
+      </c>
+      <c r="M137" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A138" t="s">
         <v>502</v>
       </c>
-      <c r="M137" t="s">
+      <c r="M138" t="s">
         <v>503</v>
-      </c>
-    </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A139" t="s">
-        <v>532</v>
-      </c>
-      <c r="M139" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A140" t="s">
+        <v>532</v>
+      </c>
+      <c r="M140" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A141" t="s">
         <v>533</v>
       </c>
-      <c r="M140" t="s">
+      <c r="M141" t="s">
         <v>534</v>
-      </c>
-    </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A142" t="s">
-        <v>605</v>
-      </c>
-      <c r="M142" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A143" t="s">
+        <v>605</v>
+      </c>
+      <c r="M143" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A144" t="s">
         <v>607</v>
       </c>
-      <c r="M143" t="s">
+      <c r="M144" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A145" t="s">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A146" t="s">
         <v>608</v>
       </c>
-      <c r="M145" t="s">
+      <c r="M146" t="s">
         <v>609</v>
-      </c>
-    </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A147" t="s">
-        <v>722</v>
-      </c>
-      <c r="M147" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A148" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="M148" t="s">
-        <v>724</v>
+        <v>733</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A149" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="M149" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A150" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="M150" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A151" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="M151" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A152" t="s">
+        <v>730</v>
+      </c>
+      <c r="M152" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A153" t="s">
         <v>731</v>
       </c>
-      <c r="M152" t="s">
+      <c r="M153" t="s">
         <v>732</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A154" t="s">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A155" t="s">
         <v>738</v>
       </c>
-      <c r="M154" t="s">
+      <c r="M155" t="s">
         <v>739</v>
-      </c>
-    </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A156" t="s">
-        <v>916</v>
-      </c>
-      <c r="M156" t="s">
-        <v>917</v>
       </c>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A157" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="M157" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A158" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="M158" t="s">
-        <v>924</v>
+        <v>919</v>
       </c>
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A159" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="M159" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A160" t="s">
+        <v>922</v>
+      </c>
+      <c r="M160" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A161" t="s">
         <v>921</v>
       </c>
-      <c r="M160" t="s">
+      <c r="M161" t="s">
         <v>923</v>
-      </c>
-    </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A162" t="s">
-        <v>981</v>
-      </c>
-      <c r="M162" t="s">
-        <v>983</v>
       </c>
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A163" t="s">
+        <v>981</v>
+      </c>
+      <c r="M163" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A164" t="s">
         <v>982</v>
       </c>
-      <c r="M163" t="s">
+      <c r="M164" t="s">
         <v>984</v>
-      </c>
-    </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A165" t="s">
-        <v>992</v>
-      </c>
-      <c r="M165" t="s">
-        <v>996</v>
       </c>
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A166" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="M166" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A167" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="M167" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A168" t="s">
+        <v>994</v>
+      </c>
+      <c r="M168" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A169" t="s">
         <v>995</v>
       </c>
-      <c r="M168" t="s">
+      <c r="M169" t="s">
         <v>999</v>
       </c>
     </row>
@@ -13359,7 +13375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445F46B3-1A86-46EF-9440-E5378C8C2CDD}">
   <dimension ref="A1:Q102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="M54" sqref="M54"/>
     </sheetView>
   </sheetViews>

</xml_diff>